<commit_message>
Auto-committed on 2022/02/16 週三
</commit_message>
<xml_diff>
--- a/Program/Other/LM051_底稿_放款資產分類案件明細表_內部控管.xlsx
+++ b/Program/Other/LM051_底稿_放款資產分類案件明細表_內部控管.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="48" windowWidth="18312" windowHeight="7608"/>
+    <workbookView xWindow="360" yWindow="50" windowWidth="18310" windowHeight="7610" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="總表" sheetId="3" r:id="rId1"/>
@@ -73,10 +73,6 @@
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
   <si>
-    <t>期數</t>
-    <phoneticPr fontId="3" type="noConversion"/>
-  </si>
-  <si>
     <t>地區別</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
@@ -375,6 +371,10 @@
   </si>
   <si>
     <t>商品代碼</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
+  <si>
+    <t>逾期數</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
 </sst>
@@ -2498,97 +2498,97 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C20" sqref="C20"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F17" sqref="F17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="21.33203125" style="37" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.77734375" style="45" customWidth="1"/>
-    <col min="3" max="3" width="21.77734375" style="46" customWidth="1"/>
-    <col min="4" max="4" width="20.109375" style="46" customWidth="1"/>
-    <col min="5" max="5" width="21.33203125" style="46" customWidth="1"/>
+    <col min="1" max="1" width="21.36328125" style="37" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.81640625" style="45" customWidth="1"/>
+    <col min="3" max="3" width="21.81640625" style="46" customWidth="1"/>
+    <col min="4" max="4" width="20.08984375" style="46" customWidth="1"/>
+    <col min="5" max="5" width="21.36328125" style="46" customWidth="1"/>
     <col min="6" max="6" width="22" style="37" customWidth="1"/>
     <col min="7" max="7" width="19" style="37" customWidth="1"/>
-    <col min="8" max="8" width="21.88671875" style="37" customWidth="1"/>
-    <col min="9" max="9" width="12.21875" style="30" customWidth="1"/>
-    <col min="10" max="10" width="25.109375" style="29" customWidth="1"/>
-    <col min="11" max="16384" width="8.88671875" style="28"/>
+    <col min="8" max="8" width="21.90625" style="37" customWidth="1"/>
+    <col min="9" max="9" width="12.1796875" style="30" customWidth="1"/>
+    <col min="10" max="10" width="25.08984375" style="29" customWidth="1"/>
+    <col min="11" max="16384" width="8.90625" style="28"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="16.8" thickBot="1" x14ac:dyDescent="0.35"/>
-    <row r="2" spans="1:10" ht="20.399999999999999" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" ht="17.5" thickBot="1" x14ac:dyDescent="0.45"/>
+    <row r="2" spans="1:10" ht="20" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A2" s="83" t="s">
+        <v>19</v>
+      </c>
+      <c r="B2" s="93" t="s">
         <v>20</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="C2" s="106" t="s">
         <v>21</v>
-      </c>
-      <c r="C2" s="106" t="s">
-        <v>22</v>
       </c>
       <c r="D2" s="107"/>
       <c r="E2" s="108" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="F2" s="109"/>
       <c r="G2" s="110"/>
       <c r="H2" s="96" t="s">
+        <v>23</v>
+      </c>
+      <c r="J2" s="36" t="s">
         <v>24</v>
       </c>
-      <c r="J2" s="36" t="s">
-        <v>25</v>
-      </c>
     </row>
-    <row r="3" spans="1:10" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A3" s="83"/>
       <c r="B3" s="94"/>
       <c r="C3" s="47" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="D3" s="48">
         <v>1.4999999999999999E-2</v>
       </c>
       <c r="E3" s="49"/>
       <c r="F3" s="47" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="G3" s="50">
         <v>0.01</v>
       </c>
       <c r="H3" s="97"/>
       <c r="J3" s="36" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
-    <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A4" s="83"/>
       <c r="B4" s="94"/>
       <c r="C4" s="87" t="s">
+        <v>28</v>
+      </c>
+      <c r="D4" s="99" t="s">
         <v>29</v>
       </c>
-      <c r="D4" s="99" t="s">
+      <c r="E4" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="E4" s="87" t="s">
+      <c r="F4" s="102" t="s">
         <v>31</v>
       </c>
-      <c r="F4" s="102" t="s">
+      <c r="G4" s="89" t="s">
         <v>32</v>
-      </c>
-      <c r="G4" s="89" t="s">
-        <v>33</v>
       </c>
       <c r="H4" s="111">
         <f>SUM(C9:G9)</f>
         <v>0</v>
       </c>
       <c r="J4" s="36" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
-    <row r="5" spans="1:10" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A5" s="83"/>
       <c r="B5" s="94"/>
       <c r="C5" s="88"/>
@@ -2598,10 +2598,10 @@
       <c r="G5" s="90"/>
       <c r="H5" s="112"/>
       <c r="J5" s="36" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
-    <row r="6" spans="1:10" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A6" s="83"/>
       <c r="B6" s="95"/>
       <c r="C6" s="98"/>
@@ -2611,13 +2611,13 @@
       <c r="G6" s="105"/>
       <c r="H6" s="112"/>
       <c r="J6" s="36" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" ht="20.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A7" s="83"/>
       <c r="B7" s="51" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C7" s="52"/>
       <c r="D7" s="22">
@@ -2634,10 +2634,10 @@
         <v>0</v>
       </c>
       <c r="J7" s="36" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
-    <row r="8" spans="1:10" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" ht="20.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A8" s="83"/>
       <c r="B8" s="56"/>
       <c r="C8" s="57"/>
@@ -2657,16 +2657,16 @@
       </c>
       <c r="I8" s="43"/>
       <c r="J8" s="36" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" ht="20.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A9" s="83"/>
       <c r="B9" s="58" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C9" s="85">
-        <f>(C7+C8)*D3</f>
+        <f>(C7+D7)*D3</f>
         <v>0</v>
       </c>
       <c r="D9" s="86"/>
@@ -2678,7 +2678,7 @@
       </c>
       <c r="H9" s="59"/>
     </row>
-    <row r="10" spans="1:10" ht="18.600000000000001" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A10" s="83"/>
       <c r="C10" s="60">
         <f>SUM(C7:D8)</f>
@@ -2691,10 +2691,10 @@
       </c>
       <c r="G10" s="63"/>
       <c r="H10" s="64" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
-    <row r="11" spans="1:10" ht="20.399999999999999" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="20" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A11" s="83"/>
       <c r="C11" s="60"/>
       <c r="D11" s="65"/>
@@ -2703,36 +2703,36 @@
         <v>0</v>
       </c>
       <c r="I11" s="40" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
-    <row r="12" spans="1:10" ht="17.399999999999999" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="18" x14ac:dyDescent="0.4">
       <c r="D12" s="61"/>
       <c r="H12" s="39"/>
       <c r="I12" s="38" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A13" s="84" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="13" spans="1:10" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="A13" s="84" t="s">
+      <c r="B13" s="66" t="s">
         <v>40</v>
       </c>
-      <c r="B13" s="66" t="s">
-        <v>41</v>
-      </c>
       <c r="E13" s="67" t="s">
+        <v>42</v>
+      </c>
+      <c r="F13" s="68" t="s">
         <v>43</v>
-      </c>
-      <c r="F13" s="68" t="s">
-        <v>44</v>
       </c>
       <c r="H13" s="69"/>
       <c r="J13" s="36"/>
     </row>
-    <row r="14" spans="1:10" ht="20.399999999999999" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" ht="20" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A14" s="83"/>
       <c r="C14" s="32" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="D14" s="31"/>
       <c r="E14" s="44">
@@ -2743,27 +2743,27 @@
       </c>
       <c r="I14" s="28"/>
       <c r="J14" s="36" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="15" spans="1:10" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A15" s="83"/>
       <c r="B15" s="70"/>
       <c r="C15" s="87" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="D15" s="89" t="s">
+        <v>44</v>
+      </c>
+      <c r="E15" s="71" t="s">
         <v>45</v>
-      </c>
-      <c r="E15" s="71" t="s">
-        <v>46</v>
       </c>
       <c r="I15" s="28"/>
       <c r="J15" s="36" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A16" s="83"/>
       <c r="B16" s="70"/>
       <c r="C16" s="88"/>
@@ -2772,10 +2772,10 @@
       <c r="F16" s="46"/>
       <c r="I16" s="28"/>
       <c r="J16" s="36" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
-    <row r="17" spans="1:10" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A17" s="83"/>
       <c r="B17" s="70"/>
       <c r="C17" s="88"/>
@@ -2784,13 +2784,13 @@
       <c r="F17" s="46"/>
       <c r="I17" s="28"/>
       <c r="J17" s="36" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
-    <row r="18" spans="1:10" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:10" ht="20.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A18" s="83"/>
       <c r="B18" s="73" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
@@ -2802,10 +2802,10 @@
       <c r="H18" s="35"/>
       <c r="I18" s="28"/>
       <c r="J18" s="34" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
-    <row r="19" spans="1:10" ht="21" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:10" ht="20.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A19" s="83"/>
       <c r="B19" s="73" t="s">
         <v>4</v>
@@ -2819,10 +2819,10 @@
       <c r="F19" s="75"/>
       <c r="I19" s="28"/>
       <c r="J19" s="34" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
-    <row r="20" spans="1:10" ht="20.399999999999999" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:10" ht="20" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A20" s="83"/>
       <c r="B20" s="73"/>
       <c r="C20" s="76">
@@ -2844,64 +2844,64 @@
       <c r="H20" s="77"/>
       <c r="I20" s="28"/>
       <c r="J20" s="34" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
-    <row r="21" spans="1:10" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
       <c r="E21" s="60"/>
       <c r="F21" s="45"/>
       <c r="J21" s="33" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="J22" s="33" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="22" spans="1:10" ht="20.399999999999999" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="J22" s="33" t="s">
+    <row r="23" spans="1:10" ht="20" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A23" s="83" t="s">
         <v>55</v>
       </c>
-    </row>
-    <row r="23" spans="1:10" ht="20.399999999999999" thickTop="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="83" t="s">
-        <v>56</v>
-      </c>
       <c r="B23" s="66" t="s">
+        <v>40</v>
+      </c>
+      <c r="C23" s="32" t="s">
         <v>41</v>
-      </c>
-      <c r="C23" s="32" t="s">
-        <v>42</v>
       </c>
       <c r="D23" s="31"/>
     </row>
-    <row r="24" spans="1:10" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
       <c r="A24" s="83"/>
       <c r="B24" s="65" t="s">
+        <v>56</v>
+      </c>
+      <c r="C24" s="91" t="s">
+        <v>28</v>
+      </c>
+      <c r="D24" s="89" t="s">
+        <v>44</v>
+      </c>
+      <c r="E24" s="71" t="s">
         <v>57</v>
       </c>
-      <c r="C24" s="91" t="s">
-        <v>29</v>
-      </c>
-      <c r="D24" s="89" t="s">
-        <v>45</v>
-      </c>
-      <c r="E24" s="71" t="s">
-        <v>58</v>
-      </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.4">
       <c r="A25" s="83"/>
       <c r="C25" s="92"/>
       <c r="D25" s="90"/>
       <c r="E25" s="72"/>
     </row>
-    <row r="26" spans="1:10" ht="16.8" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:10" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A26" s="83"/>
       <c r="C26" s="92"/>
       <c r="D26" s="90"/>
       <c r="E26" s="72"/>
     </row>
-    <row r="27" spans="1:10" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A27" s="83"/>
       <c r="B27" s="78" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C27" s="79"/>
       <c r="D27" s="80"/>
@@ -2910,10 +2910,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A28" s="83"/>
       <c r="B28" s="78" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C28" s="79"/>
       <c r="D28" s="80"/>
@@ -2922,10 +2922,10 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" ht="17.399999999999999" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
       <c r="A29" s="83"/>
       <c r="B29" s="78" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C29" s="79"/>
       <c r="D29" s="80"/>
@@ -2934,7 +2934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:10" ht="16.8" thickTop="1" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:10" ht="17.5" thickTop="1" x14ac:dyDescent="0.4">
       <c r="A30" s="83"/>
       <c r="C30" s="76">
         <f>SUM(C27:C29)</f>
@@ -2953,7 +2953,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" ht="19.8" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
       <c r="E31" s="82"/>
     </row>
   </sheetData>
@@ -2991,41 +2991,41 @@
   </sheetPr>
   <dimension ref="A1:CQ231"/>
   <sheetViews>
-    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <pane xSplit="10" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R12" sqref="R12"/>
+      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.2" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.21875" style="10" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="12.1796875" style="10" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" style="19" customWidth="1"/>
-    <col min="3" max="4" width="8.21875" style="2" customWidth="1"/>
-    <col min="5" max="5" width="19.6640625" style="3" customWidth="1"/>
-    <col min="6" max="6" width="17.6640625" style="4" customWidth="1"/>
+    <col min="3" max="4" width="8.1796875" style="2" customWidth="1"/>
+    <col min="5" max="5" width="19.6328125" style="3" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" style="4" customWidth="1"/>
     <col min="7" max="7" width="9" style="2" customWidth="1"/>
-    <col min="8" max="8" width="9" style="5" customWidth="1"/>
+    <col min="8" max="8" width="13.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.6640625" style="4" customWidth="1"/>
-    <col min="12" max="12" width="18.33203125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="16.88671875" style="4" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.08984375" style="2" customWidth="1"/>
+    <col min="11" max="11" width="15.6328125" style="4" customWidth="1"/>
+    <col min="12" max="12" width="18.36328125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="16.90625" style="4" bestFit="1" customWidth="1"/>
     <col min="14" max="14" width="17" style="4" customWidth="1"/>
-    <col min="15" max="15" width="14.21875" style="4" customWidth="1"/>
-    <col min="16" max="16" width="16.33203125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="52.33203125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="21.77734375" style="6" customWidth="1"/>
-    <col min="19" max="19" width="42.21875" style="20" customWidth="1"/>
+    <col min="15" max="15" width="14.1796875" style="4" customWidth="1"/>
+    <col min="16" max="16" width="16.36328125" style="4" customWidth="1"/>
+    <col min="17" max="17" width="52.36328125" style="3" customWidth="1"/>
+    <col min="18" max="18" width="21.81640625" style="6" customWidth="1"/>
+    <col min="19" max="19" width="42.1796875" style="20" customWidth="1"/>
     <col min="20" max="20" width="17" style="8" customWidth="1"/>
     <col min="21" max="21" width="17" style="9" customWidth="1"/>
-    <col min="22" max="22" width="12.21875" style="9" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="12.1796875" style="9" bestFit="1" customWidth="1"/>
     <col min="23" max="95" width="9" style="9"/>
     <col min="96" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" ht="19.8" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:95" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -3034,9 +3034,9 @@
       </c>
       <c r="CQ1" s="10"/>
     </row>
-    <row r="2" spans="1:95" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:95" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="18" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B2" s="11" t="s">
         <v>2</v>
@@ -3057,43 +3057,43 @@
         <v>7</v>
       </c>
       <c r="H2" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="11" t="s">
         <v>8</v>
       </c>
-      <c r="I2" s="11" t="s">
+      <c r="J2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="J2" s="11" t="s">
+      <c r="K2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="L2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="M2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="N2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="O2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="P2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="Q2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="R2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="S2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="S2" s="15" t="s">
-        <v>19</v>
-      </c>
       <c r="T2" s="16" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="U2" s="17"/>
       <c r="V2" s="17"/>
@@ -3171,7 +3171,7 @@
       <c r="CP2" s="17"/>
       <c r="CQ2" s="17"/>
     </row>
-    <row r="81" spans="2:95" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="81" spans="2:95" s="21" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B81" s="19"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
@@ -3267,7 +3267,7 @@
       <c r="CP81" s="9"/>
       <c r="CQ81" s="9"/>
     </row>
-    <row r="83" spans="2:95" s="21" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="83" spans="2:95" s="21" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B83" s="19"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
@@ -3363,7 +3363,7 @@
       <c r="CP83" s="9"/>
       <c r="CQ83" s="9"/>
     </row>
-    <row r="229" spans="2:95" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="229" spans="2:95" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B229" s="19"/>
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
@@ -3452,7 +3452,7 @@
       <c r="CP229" s="9"/>
       <c r="CQ229" s="9"/>
     </row>
-    <row r="231" spans="2:95" s="4" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="231" spans="2:95" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B231" s="19"/>
       <c r="C231" s="2"/>
       <c r="D231" s="2"/>

</xml_diff>

<commit_message>
Auto-committed on 2022/02/23 週三
</commit_message>
<xml_diff>
--- a/Program/Other/LM051_底稿_放款資產分類案件明細表_內部控管.xlsx
+++ b/Program/Other/LM051_底稿_放款資產分類案件明細表_內部控管.xlsx
@@ -16,10 +16,10 @@
     <sheet name="10804工作表" sheetId="1" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'10804工作表'!$B$2:$CF$2</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'10804工作表'!$B$2:$CG$2</definedName>
     <definedName name="_xlnm.Database" localSheetId="0">#REF!</definedName>
     <definedName name="_xlnm.Database">#REF!</definedName>
-    <definedName name="_xlnm.Print_Area" localSheetId="1">'10804工作表'!$B$1:$S$2</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="1">'10804工作表'!$B$1:$T$2</definedName>
     <definedName name="_xlnm.Print_Titles" localSheetId="1">'10804工作表'!$1:$2</definedName>
     <definedName name="新">#REF!</definedName>
   </definedNames>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="69">
   <si>
     <r>
       <t>資產分類案件明細表</t>
@@ -377,6 +377,10 @@
     <t>逾期數</t>
     <phoneticPr fontId="3" type="noConversion"/>
   </si>
+  <si>
+    <t>分類項目</t>
+    <phoneticPr fontId="3" type="noConversion"/>
+  </si>
 </sst>
 </file>
 
@@ -740,7 +744,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="35">
+  <fills count="36">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -932,6 +936,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF92D050"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="48">
     <border>
@@ -1776,7 +1786,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="113">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
@@ -2098,6 +2108,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="31" fillId="0" borderId="15" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2989,13 +3002,13 @@
     <tabColor indexed="52"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:CQ231"/>
+  <dimension ref="A1:CR231"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane xSplit="10" ySplit="2" topLeftCell="R3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="10" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="I9" sqref="I9"/>
+      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -3008,33 +3021,33 @@
     <col min="7" max="7" width="9" style="2" customWidth="1"/>
     <col min="8" max="8" width="13.7265625" style="5" bestFit="1" customWidth="1"/>
     <col min="9" max="9" width="9" style="2" customWidth="1"/>
-    <col min="10" max="10" width="13.08984375" style="2" customWidth="1"/>
-    <col min="11" max="11" width="15.6328125" style="4" customWidth="1"/>
-    <col min="12" max="12" width="18.36328125" style="4" customWidth="1"/>
-    <col min="13" max="13" width="16.90625" style="4" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="17" style="4" customWidth="1"/>
-    <col min="15" max="15" width="14.1796875" style="4" customWidth="1"/>
-    <col min="16" max="16" width="16.36328125" style="4" customWidth="1"/>
-    <col min="17" max="17" width="52.36328125" style="3" customWidth="1"/>
-    <col min="18" max="18" width="21.81640625" style="6" customWidth="1"/>
-    <col min="19" max="19" width="42.1796875" style="20" customWidth="1"/>
-    <col min="20" max="20" width="17" style="8" customWidth="1"/>
-    <col min="21" max="21" width="17" style="9" customWidth="1"/>
-    <col min="22" max="22" width="12.1796875" style="9" bestFit="1" customWidth="1"/>
-    <col min="23" max="95" width="9" style="9"/>
-    <col min="96" max="16384" width="9" style="10"/>
+    <col min="10" max="11" width="13.08984375" style="2" customWidth="1"/>
+    <col min="12" max="12" width="15.6328125" style="4" customWidth="1"/>
+    <col min="13" max="13" width="18.36328125" style="4" customWidth="1"/>
+    <col min="14" max="14" width="16.90625" style="4" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" style="4" customWidth="1"/>
+    <col min="16" max="16" width="14.1796875" style="4" customWidth="1"/>
+    <col min="17" max="17" width="16.36328125" style="4" customWidth="1"/>
+    <col min="18" max="18" width="52.36328125" style="3" customWidth="1"/>
+    <col min="19" max="19" width="21.81640625" style="6" customWidth="1"/>
+    <col min="20" max="20" width="42.1796875" style="20" customWidth="1"/>
+    <col min="21" max="21" width="17" style="8" customWidth="1"/>
+    <col min="22" max="22" width="17" style="9" customWidth="1"/>
+    <col min="23" max="23" width="12.1796875" style="9" bestFit="1" customWidth="1"/>
+    <col min="24" max="96" width="9" style="9"/>
+    <col min="97" max="16384" width="9" style="10"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:95" ht="19.5" x14ac:dyDescent="0.45">
+    <row r="1" spans="1:96" ht="19.5" x14ac:dyDescent="0.45">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="S1" s="7" t="s">
+      <c r="T1" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="CQ1" s="10"/>
+      <c r="CR1" s="10"/>
     </row>
-    <row r="2" spans="1:95" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:96" s="18" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A2" s="18" t="s">
         <v>65</v>
       </c>
@@ -3065,37 +3078,39 @@
       <c r="J2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="14" t="s">
+      <c r="K2" s="113" t="s">
+        <v>68</v>
+      </c>
+      <c r="L2" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="L2" s="14" t="s">
+      <c r="M2" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="M2" s="14" t="s">
+      <c r="N2" s="14" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="14" t="s">
+      <c r="O2" s="14" t="s">
         <v>13</v>
       </c>
-      <c r="O2" s="14" t="s">
+      <c r="P2" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="P2" s="14" t="s">
+      <c r="Q2" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="Q2" s="11" t="s">
+      <c r="R2" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="R2" s="12" t="s">
+      <c r="S2" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="S2" s="15" t="s">
+      <c r="T2" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="T2" s="16" t="s">
+      <c r="U2" s="16" t="s">
         <v>66</v>
       </c>
-      <c r="U2" s="17"/>
       <c r="V2" s="17"/>
       <c r="W2" s="17"/>
       <c r="X2" s="17"/>
@@ -3170,8 +3185,9 @@
       <c r="CO2" s="17"/>
       <c r="CP2" s="17"/>
       <c r="CQ2" s="17"/>
+      <c r="CR2" s="17"/>
     </row>
-    <row r="81" spans="2:95" s="21" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="81" spans="2:96" s="21" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B81" s="19"/>
       <c r="C81" s="2"/>
       <c r="D81" s="2"/>
@@ -3181,17 +3197,17 @@
       <c r="H81" s="5"/>
       <c r="I81" s="2"/>
       <c r="J81" s="2"/>
-      <c r="K81" s="4"/>
+      <c r="K81" s="2"/>
       <c r="L81" s="4"/>
       <c r="M81" s="4"/>
       <c r="N81" s="4"/>
       <c r="O81" s="4"/>
       <c r="P81" s="4"/>
-      <c r="Q81" s="3"/>
-      <c r="R81" s="6"/>
-      <c r="S81" s="20"/>
-      <c r="T81" s="8"/>
-      <c r="U81" s="9"/>
+      <c r="Q81" s="4"/>
+      <c r="R81" s="3"/>
+      <c r="S81" s="6"/>
+      <c r="T81" s="20"/>
+      <c r="U81" s="8"/>
       <c r="V81" s="9"/>
       <c r="W81" s="9"/>
       <c r="X81" s="9"/>
@@ -3266,8 +3282,9 @@
       <c r="CO81" s="9"/>
       <c r="CP81" s="9"/>
       <c r="CQ81" s="9"/>
+      <c r="CR81" s="9"/>
     </row>
-    <row r="83" spans="2:95" s="21" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="83" spans="2:96" s="21" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B83" s="19"/>
       <c r="C83" s="2"/>
       <c r="D83" s="2"/>
@@ -3277,17 +3294,17 @@
       <c r="H83" s="5"/>
       <c r="I83" s="2"/>
       <c r="J83" s="2"/>
-      <c r="K83" s="4"/>
+      <c r="K83" s="2"/>
       <c r="L83" s="4"/>
       <c r="M83" s="4"/>
       <c r="N83" s="4"/>
       <c r="O83" s="4"/>
       <c r="P83" s="4"/>
-      <c r="Q83" s="3"/>
-      <c r="R83" s="6"/>
-      <c r="S83" s="20"/>
-      <c r="T83" s="8"/>
-      <c r="U83" s="9"/>
+      <c r="Q83" s="4"/>
+      <c r="R83" s="3"/>
+      <c r="S83" s="6"/>
+      <c r="T83" s="20"/>
+      <c r="U83" s="8"/>
       <c r="V83" s="9"/>
       <c r="W83" s="9"/>
       <c r="X83" s="9"/>
@@ -3362,8 +3379,9 @@
       <c r="CO83" s="9"/>
       <c r="CP83" s="9"/>
       <c r="CQ83" s="9"/>
+      <c r="CR83" s="9"/>
     </row>
-    <row r="229" spans="2:95" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="229" spans="2:96" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B229" s="19"/>
       <c r="C229" s="2"/>
       <c r="D229" s="2"/>
@@ -3372,11 +3390,11 @@
       <c r="H229" s="5"/>
       <c r="I229" s="2"/>
       <c r="J229" s="2"/>
-      <c r="Q229" s="3"/>
-      <c r="R229" s="6"/>
-      <c r="S229" s="20"/>
-      <c r="T229" s="8"/>
-      <c r="U229" s="9"/>
+      <c r="K229" s="2"/>
+      <c r="R229" s="3"/>
+      <c r="S229" s="6"/>
+      <c r="T229" s="20"/>
+      <c r="U229" s="8"/>
       <c r="V229" s="9"/>
       <c r="W229" s="9"/>
       <c r="X229" s="9"/>
@@ -3451,8 +3469,9 @@
       <c r="CO229" s="9"/>
       <c r="CP229" s="9"/>
       <c r="CQ229" s="9"/>
+      <c r="CR229" s="9"/>
     </row>
-    <row r="231" spans="2:95" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="231" spans="2:96" s="4" customFormat="1" x14ac:dyDescent="0.4">
       <c r="B231" s="19"/>
       <c r="C231" s="2"/>
       <c r="D231" s="2"/>
@@ -3461,11 +3480,11 @@
       <c r="H231" s="5"/>
       <c r="I231" s="2"/>
       <c r="J231" s="2"/>
-      <c r="Q231" s="3"/>
-      <c r="R231" s="6"/>
-      <c r="S231" s="20"/>
-      <c r="T231" s="8"/>
-      <c r="U231" s="9"/>
+      <c r="K231" s="2"/>
+      <c r="R231" s="3"/>
+      <c r="S231" s="6"/>
+      <c r="T231" s="20"/>
+      <c r="U231" s="8"/>
       <c r="V231" s="9"/>
       <c r="W231" s="9"/>
       <c r="X231" s="9"/>
@@ -3540,9 +3559,10 @@
       <c r="CO231" s="9"/>
       <c r="CP231" s="9"/>
       <c r="CQ231" s="9"/>
+      <c r="CR231" s="9"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:CF2"/>
+  <autoFilter ref="B2:CG2"/>
   <phoneticPr fontId="3" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.31496062992125984" header="0.19685039370078741" footer="0.19685039370078741"/>

</xml_diff>

<commit_message>
Auto-committed on 2022/04/12 週二
</commit_message>
<xml_diff>
--- a/Program/Other/LM051_底稿_放款資產分類案件明細表_內部控管.xlsx
+++ b/Program/Other/LM051_底稿_放款資產分類案件明細表_內部控管.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="360" yWindow="50" windowWidth="18310" windowHeight="7610" activeTab="1"/>
+    <workbookView xWindow="360" yWindow="50" windowWidth="18310" windowHeight="7610"/>
   </bookViews>
   <sheets>
     <sheet name="總表" sheetId="3" r:id="rId1"/>
@@ -2020,6 +2020,72 @@
     <xf numFmtId="176" fontId="46" fillId="0" borderId="0" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="29" fillId="0" borderId="11" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="29" fillId="0" borderId="19" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="12" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="13" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="9" fillId="0" borderId="14" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="31" fillId="0" borderId="24" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="31" fillId="0" borderId="15" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" xfId="40" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2032,18 +2098,6 @@
     <xf numFmtId="176" fontId="33" fillId="0" borderId="42" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="20" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="25" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="23" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="27" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="46" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2057,60 +2111,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="28" fillId="0" borderId="19" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="29" fillId="0" borderId="11" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="29" fillId="0" borderId="19" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="28" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="21" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="29" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="22" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="26" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="30" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="31" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="12" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="13" xfId="40" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="12" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="13" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="9" fillId="0" borderId="14" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="31" fillId="0" borderId="24" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="31" fillId="0" borderId="15" xfId="40" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="35" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -2511,8 +2511,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:J31"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -2532,22 +2532,22 @@
   <sheetData>
     <row r="1" spans="1:10" ht="17.5" thickBot="1" x14ac:dyDescent="0.45"/>
     <row r="2" spans="1:10" ht="20" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="83" t="s">
+      <c r="A2" s="105" t="s">
         <v>19</v>
       </c>
-      <c r="B2" s="93" t="s">
+      <c r="B2" s="111" t="s">
         <v>20</v>
       </c>
-      <c r="C2" s="106" t="s">
+      <c r="C2" s="98" t="s">
         <v>21</v>
       </c>
-      <c r="D2" s="107"/>
-      <c r="E2" s="108" t="s">
+      <c r="D2" s="99"/>
+      <c r="E2" s="100" t="s">
         <v>22</v>
       </c>
-      <c r="F2" s="109"/>
-      <c r="G2" s="110"/>
-      <c r="H2" s="96" t="s">
+      <c r="F2" s="101"/>
+      <c r="G2" s="102"/>
+      <c r="H2" s="84" t="s">
         <v>23</v>
       </c>
       <c r="J2" s="36" t="s">
@@ -2555,8 +2555,8 @@
       </c>
     </row>
     <row r="3" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A3" s="83"/>
-      <c r="B3" s="94"/>
+      <c r="A3" s="105"/>
+      <c r="B3" s="112"/>
       <c r="C3" s="47" t="s">
         <v>25</v>
       </c>
@@ -2570,30 +2570,30 @@
       <c r="G3" s="50">
         <v>0.01</v>
       </c>
-      <c r="H3" s="97"/>
+      <c r="H3" s="85"/>
       <c r="J3" s="36" t="s">
         <v>27</v>
       </c>
     </row>
     <row r="4" spans="1:10" ht="16.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="83"/>
-      <c r="B4" s="94"/>
-      <c r="C4" s="87" t="s">
+      <c r="A4" s="105"/>
+      <c r="B4" s="112"/>
+      <c r="C4" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="D4" s="99" t="s">
+      <c r="D4" s="89" t="s">
         <v>29</v>
       </c>
-      <c r="E4" s="87" t="s">
+      <c r="E4" s="86" t="s">
         <v>30</v>
       </c>
-      <c r="F4" s="102" t="s">
+      <c r="F4" s="92" t="s">
         <v>31</v>
       </c>
-      <c r="G4" s="89" t="s">
+      <c r="G4" s="95" t="s">
         <v>32</v>
       </c>
-      <c r="H4" s="111">
+      <c r="H4" s="103">
         <f>SUM(C9:G9)</f>
         <v>0</v>
       </c>
@@ -2602,33 +2602,33 @@
       </c>
     </row>
     <row r="5" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A5" s="83"/>
-      <c r="B5" s="94"/>
-      <c r="C5" s="88"/>
-      <c r="D5" s="100"/>
-      <c r="E5" s="88"/>
-      <c r="F5" s="103"/>
-      <c r="G5" s="90"/>
-      <c r="H5" s="112"/>
+      <c r="A5" s="105"/>
+      <c r="B5" s="112"/>
+      <c r="C5" s="87"/>
+      <c r="D5" s="90"/>
+      <c r="E5" s="87"/>
+      <c r="F5" s="93"/>
+      <c r="G5" s="96"/>
+      <c r="H5" s="104"/>
       <c r="J5" s="36" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="6" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A6" s="83"/>
-      <c r="B6" s="95"/>
-      <c r="C6" s="98"/>
-      <c r="D6" s="101"/>
-      <c r="E6" s="98"/>
-      <c r="F6" s="104"/>
-      <c r="G6" s="105"/>
-      <c r="H6" s="112"/>
+      <c r="A6" s="105"/>
+      <c r="B6" s="113"/>
+      <c r="C6" s="88"/>
+      <c r="D6" s="91"/>
+      <c r="E6" s="88"/>
+      <c r="F6" s="94"/>
+      <c r="G6" s="97"/>
+      <c r="H6" s="104"/>
       <c r="J6" s="36" t="s">
         <v>63</v>
       </c>
     </row>
     <row r="7" spans="1:10" ht="20.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A7" s="83"/>
+      <c r="A7" s="105"/>
       <c r="B7" s="51" t="s">
         <v>34</v>
       </c>
@@ -2643,7 +2643,7 @@
         <v>0</v>
       </c>
       <c r="H7" s="55">
-        <f>SUM(E7:G7)*G3+(C7*D3)</f>
+        <f>SUM(E7:G7)*G3+((C7+D7)*D3)</f>
         <v>0</v>
       </c>
       <c r="J7" s="36" t="s">
@@ -2651,7 +2651,7 @@
       </c>
     </row>
     <row r="8" spans="1:10" ht="20.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A8" s="83"/>
+      <c r="A8" s="105"/>
       <c r="B8" s="56"/>
       <c r="C8" s="57"/>
       <c r="D8" s="24"/>
@@ -2674,15 +2674,15 @@
       </c>
     </row>
     <row r="9" spans="1:10" ht="20.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A9" s="83"/>
+      <c r="A9" s="105"/>
       <c r="B9" s="58" t="s">
         <v>35</v>
       </c>
-      <c r="C9" s="85">
+      <c r="C9" s="107">
         <f>(C7+D7)*D3</f>
         <v>0</v>
       </c>
-      <c r="D9" s="86"/>
+      <c r="D9" s="108"/>
       <c r="E9" s="42"/>
       <c r="F9" s="41"/>
       <c r="G9" s="26">
@@ -2692,7 +2692,7 @@
       <c r="H9" s="59"/>
     </row>
     <row r="10" spans="1:10" ht="18.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A10" s="83"/>
+      <c r="A10" s="105"/>
       <c r="C10" s="60">
         <f>SUM(C7:D8)</f>
         <v>0</v>
@@ -2708,7 +2708,7 @@
       </c>
     </row>
     <row r="11" spans="1:10" ht="20" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="83"/>
+      <c r="A11" s="105"/>
       <c r="C11" s="60"/>
       <c r="D11" s="65"/>
       <c r="H11" s="35">
@@ -2727,7 +2727,7 @@
       </c>
     </row>
     <row r="13" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A13" s="84" t="s">
+      <c r="A13" s="106" t="s">
         <v>39</v>
       </c>
       <c r="B13" s="66" t="s">
@@ -2743,7 +2743,7 @@
       <c r="J13" s="36"/>
     </row>
     <row r="14" spans="1:10" ht="20" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="83"/>
+      <c r="A14" s="105"/>
       <c r="C14" s="32" t="s">
         <v>41</v>
       </c>
@@ -2760,12 +2760,12 @@
       </c>
     </row>
     <row r="15" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A15" s="83"/>
+      <c r="A15" s="105"/>
       <c r="B15" s="70"/>
-      <c r="C15" s="87" t="s">
+      <c r="C15" s="86" t="s">
         <v>28</v>
       </c>
-      <c r="D15" s="89" t="s">
+      <c r="D15" s="95" t="s">
         <v>44</v>
       </c>
       <c r="E15" s="71" t="s">
@@ -2777,10 +2777,10 @@
       </c>
     </row>
     <row r="16" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A16" s="83"/>
+      <c r="A16" s="105"/>
       <c r="B16" s="70"/>
-      <c r="C16" s="88"/>
-      <c r="D16" s="90"/>
+      <c r="C16" s="87"/>
+      <c r="D16" s="96"/>
       <c r="E16" s="72"/>
       <c r="F16" s="46"/>
       <c r="I16" s="28"/>
@@ -2789,10 +2789,10 @@
       </c>
     </row>
     <row r="17" spans="1:10" ht="20" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A17" s="83"/>
+      <c r="A17" s="105"/>
       <c r="B17" s="70"/>
-      <c r="C17" s="88"/>
-      <c r="D17" s="90"/>
+      <c r="C17" s="87"/>
+      <c r="D17" s="96"/>
       <c r="E17" s="72"/>
       <c r="F17" s="46"/>
       <c r="I17" s="28"/>
@@ -2801,7 +2801,7 @@
       </c>
     </row>
     <row r="18" spans="1:10" ht="20.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A18" s="83"/>
+      <c r="A18" s="105"/>
       <c r="B18" s="73" t="s">
         <v>49</v>
       </c>
@@ -2819,7 +2819,7 @@
       </c>
     </row>
     <row r="19" spans="1:10" ht="20.5" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A19" s="83"/>
+      <c r="A19" s="105"/>
       <c r="B19" s="73" t="s">
         <v>4</v>
       </c>
@@ -2836,7 +2836,7 @@
       </c>
     </row>
     <row r="20" spans="1:10" ht="20" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A20" s="83"/>
+      <c r="A20" s="105"/>
       <c r="B20" s="73"/>
       <c r="C20" s="76">
         <f>SUM(C18:C19)</f>
@@ -2873,7 +2873,7 @@
       </c>
     </row>
     <row r="23" spans="1:10" ht="20" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="83" t="s">
+      <c r="A23" s="105" t="s">
         <v>55</v>
       </c>
       <c r="B23" s="66" t="s">
@@ -2885,14 +2885,14 @@
       <c r="D23" s="31"/>
     </row>
     <row r="24" spans="1:10" ht="19.5" x14ac:dyDescent="0.4">
-      <c r="A24" s="83"/>
+      <c r="A24" s="105"/>
       <c r="B24" s="65" t="s">
         <v>56</v>
       </c>
-      <c r="C24" s="91" t="s">
+      <c r="C24" s="109" t="s">
         <v>28</v>
       </c>
-      <c r="D24" s="89" t="s">
+      <c r="D24" s="95" t="s">
         <v>44</v>
       </c>
       <c r="E24" s="71" t="s">
@@ -2900,19 +2900,19 @@
       </c>
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.4">
-      <c r="A25" s="83"/>
-      <c r="C25" s="92"/>
-      <c r="D25" s="90"/>
+      <c r="A25" s="105"/>
+      <c r="C25" s="110"/>
+      <c r="D25" s="96"/>
       <c r="E25" s="72"/>
     </row>
     <row r="26" spans="1:10" ht="17.5" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A26" s="83"/>
-      <c r="C26" s="92"/>
-      <c r="D26" s="90"/>
+      <c r="A26" s="105"/>
+      <c r="C26" s="110"/>
+      <c r="D26" s="96"/>
       <c r="E26" s="72"/>
     </row>
     <row r="27" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A27" s="83"/>
+      <c r="A27" s="105"/>
       <c r="B27" s="78" t="s">
         <v>58</v>
       </c>
@@ -2924,7 +2924,7 @@
       </c>
     </row>
     <row r="28" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="83"/>
+      <c r="A28" s="105"/>
       <c r="B28" s="78" t="s">
         <v>59</v>
       </c>
@@ -2936,7 +2936,7 @@
       </c>
     </row>
     <row r="29" spans="1:10" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="83"/>
+      <c r="A29" s="105"/>
       <c r="B29" s="78" t="s">
         <v>60</v>
       </c>
@@ -2948,7 +2948,7 @@
       </c>
     </row>
     <row r="30" spans="1:10" ht="17.5" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="83"/>
+      <c r="A30" s="105"/>
       <c r="C30" s="76">
         <f>SUM(C27:C29)</f>
         <v>0</v>
@@ -2971,6 +2971,15 @@
     </row>
   </sheetData>
   <mergeCells count="18">
+    <mergeCell ref="A2:A11"/>
+    <mergeCell ref="A13:A20"/>
+    <mergeCell ref="A23:A30"/>
+    <mergeCell ref="C9:D9"/>
+    <mergeCell ref="C15:C17"/>
+    <mergeCell ref="D15:D17"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="D24:D26"/>
+    <mergeCell ref="B2:B6"/>
     <mergeCell ref="H2:H3"/>
     <mergeCell ref="C4:C6"/>
     <mergeCell ref="D4:D6"/>
@@ -2980,15 +2989,6 @@
     <mergeCell ref="C2:D2"/>
     <mergeCell ref="E2:G2"/>
     <mergeCell ref="H4:H6"/>
-    <mergeCell ref="A2:A11"/>
-    <mergeCell ref="A13:A20"/>
-    <mergeCell ref="A23:A30"/>
-    <mergeCell ref="C9:D9"/>
-    <mergeCell ref="C15:C17"/>
-    <mergeCell ref="D15:D17"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="D24:D26"/>
-    <mergeCell ref="B2:B6"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3004,11 +3004,11 @@
   </sheetPr>
   <dimension ref="A1:CR231"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <pane xSplit="10" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="G9" sqref="G9"/>
+      <selection pane="bottomRight" activeCell="B22" sqref="B22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
@@ -3078,7 +3078,7 @@
       <c r="J2" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="K2" s="113" t="s">
+      <c r="K2" s="83" t="s">
         <v>68</v>
       </c>
       <c r="L2" s="14" t="s">

</xml_diff>

<commit_message>
Auto-committed on 2023/04/24 週一 11:29:32.75
</commit_message>
<xml_diff>
--- a/Program/Other/LM051_底稿_放款資產分類案件明細表_內部控管.xlsx
+++ b/Program/Other/LM051_底稿_放款資產分類案件明細表_內部控管.xlsx
@@ -1,23 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="26227"/>
   <workbookPr codeName="ThisWorkbook" hidePivotFieldList="1"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\192.168.10.8\itxDoc\itxWrite\excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\SVN\iTX\Other\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8650AE56-C3D4-4036-BEDD-7B0F801DA72B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14420" windowHeight="6110" tabRatio="901" activeTab="1"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11020" tabRatio="901" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="備呆總表" sheetId="58" r:id="rId1"/>
     <sheet name="10804工作表" sheetId="61" r:id="rId2"/>
   </sheets>
-  <externalReferences>
-    <externalReference r:id="rId3"/>
-  </externalReferences>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="1" hidden="1">'10804工作表'!$B$2:$CG$2</definedName>
     <definedName name="_xlnm.Database" localSheetId="1">#REF!</definedName>
@@ -29,17 +27,17 @@
     <definedName name="新" localSheetId="1">#REF!</definedName>
     <definedName name="新">#REF!</definedName>
   </definedNames>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>A satisfied Microsoft Office User</author>
   </authors>
   <commentList>
-    <comment ref="U12" authorId="0" shapeId="0">
+    <comment ref="U12" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -53,7 +51,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="U13" authorId="0" shapeId="0">
+    <comment ref="U13" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000002000000}">
       <text>
         <r>
           <rPr>
@@ -67,7 +65,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="C17" authorId="0" shapeId="0">
+    <comment ref="C17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000003000000}">
       <text>
         <r>
           <rPr>
@@ -82,7 +80,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D17" authorId="0" shapeId="0">
+    <comment ref="D17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000004000000}">
       <text>
         <r>
           <rPr>
@@ -97,7 +95,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F17" authorId="0" shapeId="0">
+    <comment ref="F17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000005000000}">
       <text>
         <r>
           <rPr>
@@ -112,7 +110,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="G17" authorId="0" shapeId="0">
+    <comment ref="G17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000006000000}">
       <text>
         <r>
           <rPr>
@@ -127,7 +125,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="H17" authorId="0" shapeId="0">
+    <comment ref="H17" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000007000000}">
       <text>
         <r>
           <rPr>
@@ -634,7 +632,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="10">
     <numFmt numFmtId="41" formatCode="_-* #,##0_-;\-* #,##0_-;_-* &quot;-&quot;_-;_-@_-"/>
     <numFmt numFmtId="43" formatCode="_-* #,##0.00_-;\-* #,##0.00_-;_-* &quot;-&quot;??_-;_-@_-"/>
@@ -3181,21 +3179,21 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="323">
+  <cellXfs count="308">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="177" fontId="7" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="10" fillId="0" borderId="0" xfId="93" applyFont="1" applyAlignment="1">
@@ -3210,12 +3208,6 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" xfId="93" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3234,13 +3226,13 @@
     <xf numFmtId="182" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="9" fillId="0" borderId="0" xfId="93" applyFont="1" applyAlignment="1">
@@ -3255,7 +3247,7 @@
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3276,7 +3268,7 @@
     <xf numFmtId="177" fontId="19" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="49" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3286,9 +3278,6 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="50" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3300,9 +3289,6 @@
     <xf numFmtId="9" fontId="51" fillId="0" borderId="0" xfId="93" applyFont="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3315,37 +3301,37 @@
     <xf numFmtId="9" fontId="23" fillId="0" borderId="0" xfId="93" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="52" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="53" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="8" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="54" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="55" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="55" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="15" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3354,13 +3340,10 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="16" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="57" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="57" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3387,34 +3370,31 @@
     <xf numFmtId="1" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="60" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="56" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="183" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="60" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="183" fontId="59" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="20" fillId="0" borderId="0" xfId="93" applyFont="1" applyAlignment="1">
@@ -3426,21 +3406,15 @@
     <xf numFmtId="176" fontId="63" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="183" fontId="58" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="58" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="50" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
     <xf numFmtId="176" fontId="28" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -3459,40 +3433,37 @@
     <xf numFmtId="176" fontId="65" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="176" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="61" fillId="0" borderId="26" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="61" fillId="0" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="61" fillId="0" borderId="27" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="10" fontId="61" fillId="0" borderId="27" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="30" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="67" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -3507,10 +3478,10 @@
     <xf numFmtId="176" fontId="19" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
     <xf numFmtId="181" fontId="19" fillId="0" borderId="12" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3555,10 +3526,10 @@
     <xf numFmtId="176" fontId="4" fillId="0" borderId="13" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="4" fillId="0" borderId="15" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -3576,7 +3547,7 @@
     <xf numFmtId="0" fontId="72" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="73" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="74" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3606,13 +3577,13 @@
     <xf numFmtId="176" fontId="76" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="76" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="76" fillId="0" borderId="0" xfId="76" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="77" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="43" fontId="4" fillId="0" borderId="21" xfId="76" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3621,40 +3592,40 @@
     <xf numFmtId="176" fontId="69" fillId="0" borderId="9" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="43" fontId="78" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="43" fontId="78" fillId="0" borderId="0" xfId="76" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="180" fontId="4" fillId="0" borderId="22" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="79" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="79" fillId="0" borderId="0" xfId="76" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="76" fillId="0" borderId="0" xfId="93" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="19" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="80" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="55" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="55" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="80" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="81" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyAlignment="1">
@@ -3675,7 +3646,7 @@
     <xf numFmtId="10" fontId="61" fillId="0" borderId="27" xfId="93" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
-    <xf numFmtId="181" fontId="61" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="181" fontId="61" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
     <xf numFmtId="9" fontId="84" fillId="0" borderId="0" xfId="93" applyFont="1" applyFill="1" applyAlignment="1">
@@ -3699,22 +3670,360 @@
     <xf numFmtId="176" fontId="31" fillId="0" borderId="34" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="177" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="61" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="177" fontId="31" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="61" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="176" fontId="61" fillId="0" borderId="35" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" indent="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="31" fillId="35" borderId="2" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="36" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="25" fillId="36" borderId="2" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="31" fillId="36" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="176" fontId="64" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="31" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="66" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="66" fillId="0" borderId="67" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="61" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="61" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="15" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="21" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="10" fontId="4" fillId="0" borderId="33" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="25" fillId="0" borderId="31" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="25" fillId="0" borderId="62" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="54" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="24" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="179" fontId="4" fillId="0" borderId="55" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="60" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="61" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="21" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="48" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="83" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="83" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="83" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="61" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="61" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="66" fillId="0" borderId="66" xfId="93" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="9" fontId="66" fillId="0" borderId="67" xfId="93" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="60" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="77" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="78" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="70" fillId="0" borderId="32" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="70" fillId="0" borderId="82" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="83" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="84" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="19" fillId="0" borderId="85" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="21" xfId="79" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="178" fontId="4" fillId="0" borderId="48" xfId="79" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="21" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="4" fillId="0" borderId="48" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="68" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="69" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="70" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="21" xfId="76" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="48" xfId="76" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" indent="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="36" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="177" fontId="4" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="9" fontId="29" fillId="0" borderId="0" xfId="93" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="26" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="31" fillId="0" borderId="15" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3723,31 +4032,31 @@
     <xf numFmtId="176" fontId="31" fillId="0" borderId="86" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="37" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="38" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="180" fontId="4" fillId="0" borderId="39" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="40" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="41" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="42" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="43" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="176" fontId="66" fillId="0" borderId="16" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -3756,562 +4065,210 @@
     <xf numFmtId="176" fontId="66" fillId="0" borderId="28" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="44" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="45" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="45" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="31" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="50" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="51" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="52" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="53" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="21" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="48" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="72" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="75" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="73" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="40" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="42" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="43" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="21" xfId="76" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="4" fillId="0" borderId="48" xfId="76" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="71" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="49" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="63" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="64" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="65" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="79" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="80" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="29" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="27" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1" indent="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="48" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="46" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="44" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="33" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="43" fontId="83" fillId="0" borderId="74" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="83" fillId="0" borderId="75" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="83" fillId="0" borderId="76" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="61" fillId="0" borderId="16" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="61" fillId="0" borderId="28" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="66" fillId="0" borderId="66" xfId="93" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="9" fontId="66" fillId="0" borderId="67" xfId="93" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="60" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="77" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="180" fontId="4" fillId="0" borderId="78" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="79" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="80" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="17" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="29" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="19" fillId="0" borderId="20" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="81" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="48" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="70" fillId="0" borderId="32" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="70" fillId="0" borderId="82" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="19" fillId="0" borderId="83" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="19" fillId="0" borderId="84" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="19" fillId="0" borderId="85" xfId="76" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="21" xfId="79" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="4" fillId="0" borderId="48" xfId="79" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="21" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="4" fillId="0" borderId="48" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="68" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="69" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="70" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="177" fontId="4" fillId="0" borderId="21" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="48" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="21" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="10" fontId="4" fillId="0" borderId="33" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="25" fillId="0" borderId="31" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="25" fillId="0" borderId="62" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="66" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="66" fillId="0" borderId="67" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="54" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="24" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="179" fontId="4" fillId="0" borderId="55" xfId="93" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center" indent="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="56" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="60" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="61" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="37" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="19" fillId="0" borderId="47" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="64" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="31" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="0" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="61" fillId="0" borderId="72" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="61" fillId="0" borderId="73" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="57" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="58" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="177" fontId="15" fillId="0" borderId="59" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left" indent="1"/>
-    </xf>
-    <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="178" fontId="6" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="31" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="35" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="31" fillId="35" borderId="2" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="36" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="25" fillId="36" borderId="2" xfId="76" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="31" fillId="37" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="178" fontId="31" fillId="36" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="85" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="86" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="175">
-    <cellStyle name="20% - 輔色1 2" xfId="1"/>
-    <cellStyle name="20% - 輔色1 2 2" xfId="2"/>
-    <cellStyle name="20% - 輔色1 3" xfId="3"/>
-    <cellStyle name="20% - 輔色1 3 2" xfId="4"/>
-    <cellStyle name="20% - 輔色2 2" xfId="5"/>
-    <cellStyle name="20% - 輔色2 2 2" xfId="6"/>
-    <cellStyle name="20% - 輔色2 3" xfId="7"/>
-    <cellStyle name="20% - 輔色2 3 2" xfId="8"/>
-    <cellStyle name="20% - 輔色3 2" xfId="9"/>
-    <cellStyle name="20% - 輔色3 2 2" xfId="10"/>
-    <cellStyle name="20% - 輔色3 3" xfId="11"/>
-    <cellStyle name="20% - 輔色3 3 2" xfId="12"/>
-    <cellStyle name="20% - 輔色4 2" xfId="13"/>
-    <cellStyle name="20% - 輔色4 2 2" xfId="14"/>
-    <cellStyle name="20% - 輔色4 3" xfId="15"/>
-    <cellStyle name="20% - 輔色4 3 2" xfId="16"/>
-    <cellStyle name="20% - 輔色5 2" xfId="17"/>
-    <cellStyle name="20% - 輔色5 2 2" xfId="18"/>
-    <cellStyle name="20% - 輔色5 3" xfId="19"/>
-    <cellStyle name="20% - 輔色5 3 2" xfId="20"/>
-    <cellStyle name="20% - 輔色6 2" xfId="21"/>
-    <cellStyle name="20% - 輔色6 2 2" xfId="22"/>
-    <cellStyle name="20% - 輔色6 3" xfId="23"/>
-    <cellStyle name="20% - 輔色6 3 2" xfId="24"/>
-    <cellStyle name="40% - 輔色1 2" xfId="25"/>
-    <cellStyle name="40% - 輔色1 2 2" xfId="26"/>
-    <cellStyle name="40% - 輔色1 3" xfId="27"/>
-    <cellStyle name="40% - 輔色1 3 2" xfId="28"/>
-    <cellStyle name="40% - 輔色2 2" xfId="29"/>
-    <cellStyle name="40% - 輔色2 2 2" xfId="30"/>
-    <cellStyle name="40% - 輔色2 3" xfId="31"/>
-    <cellStyle name="40% - 輔色2 3 2" xfId="32"/>
-    <cellStyle name="40% - 輔色3 2" xfId="33"/>
-    <cellStyle name="40% - 輔色3 2 2" xfId="34"/>
-    <cellStyle name="40% - 輔色3 3" xfId="35"/>
-    <cellStyle name="40% - 輔色3 3 2" xfId="36"/>
-    <cellStyle name="40% - 輔色4 2" xfId="37"/>
-    <cellStyle name="40% - 輔色4 2 2" xfId="38"/>
-    <cellStyle name="40% - 輔色4 3" xfId="39"/>
-    <cellStyle name="40% - 輔色4 3 2" xfId="40"/>
-    <cellStyle name="40% - 輔色5 2" xfId="41"/>
-    <cellStyle name="40% - 輔色5 2 2" xfId="42"/>
-    <cellStyle name="40% - 輔色5 3" xfId="43"/>
-    <cellStyle name="40% - 輔色5 3 2" xfId="44"/>
-    <cellStyle name="40% - 輔色6 2" xfId="45"/>
-    <cellStyle name="40% - 輔色6 2 2" xfId="46"/>
-    <cellStyle name="40% - 輔色6 3" xfId="47"/>
-    <cellStyle name="40% - 輔色6 3 2" xfId="48"/>
-    <cellStyle name="60% - 輔色1 2" xfId="49"/>
-    <cellStyle name="60% - 輔色1 2 2" xfId="50"/>
-    <cellStyle name="60% - 輔色1 3" xfId="51"/>
-    <cellStyle name="60% - 輔色1 3 2" xfId="52"/>
-    <cellStyle name="60% - 輔色2 2" xfId="53"/>
-    <cellStyle name="60% - 輔色2 2 2" xfId="54"/>
-    <cellStyle name="60% - 輔色2 3" xfId="55"/>
-    <cellStyle name="60% - 輔色2 3 2" xfId="56"/>
-    <cellStyle name="60% - 輔色3 2" xfId="57"/>
-    <cellStyle name="60% - 輔色3 2 2" xfId="58"/>
-    <cellStyle name="60% - 輔色3 3" xfId="59"/>
-    <cellStyle name="60% - 輔色3 3 2" xfId="60"/>
-    <cellStyle name="60% - 輔色4 2" xfId="61"/>
-    <cellStyle name="60% - 輔色4 2 2" xfId="62"/>
-    <cellStyle name="60% - 輔色4 3" xfId="63"/>
-    <cellStyle name="60% - 輔色4 3 2" xfId="64"/>
-    <cellStyle name="60% - 輔色5 2" xfId="65"/>
-    <cellStyle name="60% - 輔色5 2 2" xfId="66"/>
-    <cellStyle name="60% - 輔色5 3" xfId="67"/>
-    <cellStyle name="60% - 輔色5 3 2" xfId="68"/>
-    <cellStyle name="60% - 輔色6 2" xfId="69"/>
-    <cellStyle name="60% - 輔色6 2 2" xfId="70"/>
-    <cellStyle name="60% - 輔色6 3" xfId="71"/>
-    <cellStyle name="60% - 輔色6 3 2" xfId="72"/>
+    <cellStyle name="20% - 輔色1 2" xfId="1" xr:uid="{00000000-0005-0000-0000-000000000000}"/>
+    <cellStyle name="20% - 輔色1 2 2" xfId="2" xr:uid="{00000000-0005-0000-0000-000001000000}"/>
+    <cellStyle name="20% - 輔色1 3" xfId="3" xr:uid="{00000000-0005-0000-0000-000002000000}"/>
+    <cellStyle name="20% - 輔色1 3 2" xfId="4" xr:uid="{00000000-0005-0000-0000-000003000000}"/>
+    <cellStyle name="20% - 輔色2 2" xfId="5" xr:uid="{00000000-0005-0000-0000-000004000000}"/>
+    <cellStyle name="20% - 輔色2 2 2" xfId="6" xr:uid="{00000000-0005-0000-0000-000005000000}"/>
+    <cellStyle name="20% - 輔色2 3" xfId="7" xr:uid="{00000000-0005-0000-0000-000006000000}"/>
+    <cellStyle name="20% - 輔色2 3 2" xfId="8" xr:uid="{00000000-0005-0000-0000-000007000000}"/>
+    <cellStyle name="20% - 輔色3 2" xfId="9" xr:uid="{00000000-0005-0000-0000-000008000000}"/>
+    <cellStyle name="20% - 輔色3 2 2" xfId="10" xr:uid="{00000000-0005-0000-0000-000009000000}"/>
+    <cellStyle name="20% - 輔色3 3" xfId="11" xr:uid="{00000000-0005-0000-0000-00000A000000}"/>
+    <cellStyle name="20% - 輔色3 3 2" xfId="12" xr:uid="{00000000-0005-0000-0000-00000B000000}"/>
+    <cellStyle name="20% - 輔色4 2" xfId="13" xr:uid="{00000000-0005-0000-0000-00000C000000}"/>
+    <cellStyle name="20% - 輔色4 2 2" xfId="14" xr:uid="{00000000-0005-0000-0000-00000D000000}"/>
+    <cellStyle name="20% - 輔色4 3" xfId="15" xr:uid="{00000000-0005-0000-0000-00000E000000}"/>
+    <cellStyle name="20% - 輔色4 3 2" xfId="16" xr:uid="{00000000-0005-0000-0000-00000F000000}"/>
+    <cellStyle name="20% - 輔色5 2" xfId="17" xr:uid="{00000000-0005-0000-0000-000010000000}"/>
+    <cellStyle name="20% - 輔色5 2 2" xfId="18" xr:uid="{00000000-0005-0000-0000-000011000000}"/>
+    <cellStyle name="20% - 輔色5 3" xfId="19" xr:uid="{00000000-0005-0000-0000-000012000000}"/>
+    <cellStyle name="20% - 輔色5 3 2" xfId="20" xr:uid="{00000000-0005-0000-0000-000013000000}"/>
+    <cellStyle name="20% - 輔色6 2" xfId="21" xr:uid="{00000000-0005-0000-0000-000014000000}"/>
+    <cellStyle name="20% - 輔色6 2 2" xfId="22" xr:uid="{00000000-0005-0000-0000-000015000000}"/>
+    <cellStyle name="20% - 輔色6 3" xfId="23" xr:uid="{00000000-0005-0000-0000-000016000000}"/>
+    <cellStyle name="20% - 輔色6 3 2" xfId="24" xr:uid="{00000000-0005-0000-0000-000017000000}"/>
+    <cellStyle name="40% - 輔色1 2" xfId="25" xr:uid="{00000000-0005-0000-0000-000018000000}"/>
+    <cellStyle name="40% - 輔色1 2 2" xfId="26" xr:uid="{00000000-0005-0000-0000-000019000000}"/>
+    <cellStyle name="40% - 輔色1 3" xfId="27" xr:uid="{00000000-0005-0000-0000-00001A000000}"/>
+    <cellStyle name="40% - 輔色1 3 2" xfId="28" xr:uid="{00000000-0005-0000-0000-00001B000000}"/>
+    <cellStyle name="40% - 輔色2 2" xfId="29" xr:uid="{00000000-0005-0000-0000-00001C000000}"/>
+    <cellStyle name="40% - 輔色2 2 2" xfId="30" xr:uid="{00000000-0005-0000-0000-00001D000000}"/>
+    <cellStyle name="40% - 輔色2 3" xfId="31" xr:uid="{00000000-0005-0000-0000-00001E000000}"/>
+    <cellStyle name="40% - 輔色2 3 2" xfId="32" xr:uid="{00000000-0005-0000-0000-00001F000000}"/>
+    <cellStyle name="40% - 輔色3 2" xfId="33" xr:uid="{00000000-0005-0000-0000-000020000000}"/>
+    <cellStyle name="40% - 輔色3 2 2" xfId="34" xr:uid="{00000000-0005-0000-0000-000021000000}"/>
+    <cellStyle name="40% - 輔色3 3" xfId="35" xr:uid="{00000000-0005-0000-0000-000022000000}"/>
+    <cellStyle name="40% - 輔色3 3 2" xfId="36" xr:uid="{00000000-0005-0000-0000-000023000000}"/>
+    <cellStyle name="40% - 輔色4 2" xfId="37" xr:uid="{00000000-0005-0000-0000-000024000000}"/>
+    <cellStyle name="40% - 輔色4 2 2" xfId="38" xr:uid="{00000000-0005-0000-0000-000025000000}"/>
+    <cellStyle name="40% - 輔色4 3" xfId="39" xr:uid="{00000000-0005-0000-0000-000026000000}"/>
+    <cellStyle name="40% - 輔色4 3 2" xfId="40" xr:uid="{00000000-0005-0000-0000-000027000000}"/>
+    <cellStyle name="40% - 輔色5 2" xfId="41" xr:uid="{00000000-0005-0000-0000-000028000000}"/>
+    <cellStyle name="40% - 輔色5 2 2" xfId="42" xr:uid="{00000000-0005-0000-0000-000029000000}"/>
+    <cellStyle name="40% - 輔色5 3" xfId="43" xr:uid="{00000000-0005-0000-0000-00002A000000}"/>
+    <cellStyle name="40% - 輔色5 3 2" xfId="44" xr:uid="{00000000-0005-0000-0000-00002B000000}"/>
+    <cellStyle name="40% - 輔色6 2" xfId="45" xr:uid="{00000000-0005-0000-0000-00002C000000}"/>
+    <cellStyle name="40% - 輔色6 2 2" xfId="46" xr:uid="{00000000-0005-0000-0000-00002D000000}"/>
+    <cellStyle name="40% - 輔色6 3" xfId="47" xr:uid="{00000000-0005-0000-0000-00002E000000}"/>
+    <cellStyle name="40% - 輔色6 3 2" xfId="48" xr:uid="{00000000-0005-0000-0000-00002F000000}"/>
+    <cellStyle name="60% - 輔色1 2" xfId="49" xr:uid="{00000000-0005-0000-0000-000030000000}"/>
+    <cellStyle name="60% - 輔色1 2 2" xfId="50" xr:uid="{00000000-0005-0000-0000-000031000000}"/>
+    <cellStyle name="60% - 輔色1 3" xfId="51" xr:uid="{00000000-0005-0000-0000-000032000000}"/>
+    <cellStyle name="60% - 輔色1 3 2" xfId="52" xr:uid="{00000000-0005-0000-0000-000033000000}"/>
+    <cellStyle name="60% - 輔色2 2" xfId="53" xr:uid="{00000000-0005-0000-0000-000034000000}"/>
+    <cellStyle name="60% - 輔色2 2 2" xfId="54" xr:uid="{00000000-0005-0000-0000-000035000000}"/>
+    <cellStyle name="60% - 輔色2 3" xfId="55" xr:uid="{00000000-0005-0000-0000-000036000000}"/>
+    <cellStyle name="60% - 輔色2 3 2" xfId="56" xr:uid="{00000000-0005-0000-0000-000037000000}"/>
+    <cellStyle name="60% - 輔色3 2" xfId="57" xr:uid="{00000000-0005-0000-0000-000038000000}"/>
+    <cellStyle name="60% - 輔色3 2 2" xfId="58" xr:uid="{00000000-0005-0000-0000-000039000000}"/>
+    <cellStyle name="60% - 輔色3 3" xfId="59" xr:uid="{00000000-0005-0000-0000-00003A000000}"/>
+    <cellStyle name="60% - 輔色3 3 2" xfId="60" xr:uid="{00000000-0005-0000-0000-00003B000000}"/>
+    <cellStyle name="60% - 輔色4 2" xfId="61" xr:uid="{00000000-0005-0000-0000-00003C000000}"/>
+    <cellStyle name="60% - 輔色4 2 2" xfId="62" xr:uid="{00000000-0005-0000-0000-00003D000000}"/>
+    <cellStyle name="60% - 輔色4 3" xfId="63" xr:uid="{00000000-0005-0000-0000-00003E000000}"/>
+    <cellStyle name="60% - 輔色4 3 2" xfId="64" xr:uid="{00000000-0005-0000-0000-00003F000000}"/>
+    <cellStyle name="60% - 輔色5 2" xfId="65" xr:uid="{00000000-0005-0000-0000-000040000000}"/>
+    <cellStyle name="60% - 輔色5 2 2" xfId="66" xr:uid="{00000000-0005-0000-0000-000041000000}"/>
+    <cellStyle name="60% - 輔色5 3" xfId="67" xr:uid="{00000000-0005-0000-0000-000042000000}"/>
+    <cellStyle name="60% - 輔色5 3 2" xfId="68" xr:uid="{00000000-0005-0000-0000-000043000000}"/>
+    <cellStyle name="60% - 輔色6 2" xfId="69" xr:uid="{00000000-0005-0000-0000-000044000000}"/>
+    <cellStyle name="60% - 輔色6 2 2" xfId="70" xr:uid="{00000000-0005-0000-0000-000045000000}"/>
+    <cellStyle name="60% - 輔色6 3" xfId="71" xr:uid="{00000000-0005-0000-0000-000046000000}"/>
+    <cellStyle name="60% - 輔色6 3 2" xfId="72" xr:uid="{00000000-0005-0000-0000-000047000000}"/>
     <cellStyle name="一般" xfId="0" builtinId="0"/>
-    <cellStyle name="一般 2 2" xfId="73"/>
-    <cellStyle name="一般 3 2" xfId="74"/>
-    <cellStyle name="一般 4" xfId="75"/>
+    <cellStyle name="一般 2 2" xfId="73" xr:uid="{00000000-0005-0000-0000-000049000000}"/>
+    <cellStyle name="一般 3 2" xfId="74" xr:uid="{00000000-0005-0000-0000-00004A000000}"/>
+    <cellStyle name="一般 4" xfId="75" xr:uid="{00000000-0005-0000-0000-00004B000000}"/>
     <cellStyle name="千分位" xfId="76" builtinId="3"/>
-    <cellStyle name="千分位 2" xfId="77"/>
-    <cellStyle name="千分位 3" xfId="78"/>
+    <cellStyle name="千分位 2" xfId="77" xr:uid="{00000000-0005-0000-0000-00004D000000}"/>
+    <cellStyle name="千分位 3" xfId="78" xr:uid="{00000000-0005-0000-0000-00004E000000}"/>
     <cellStyle name="千分位[0]" xfId="79" builtinId="6"/>
-    <cellStyle name="千分位[0] 2" xfId="80"/>
-    <cellStyle name="中等 2" xfId="81"/>
-    <cellStyle name="中等 2 2" xfId="82"/>
-    <cellStyle name="中等 3" xfId="83"/>
-    <cellStyle name="中等 3 2" xfId="84"/>
-    <cellStyle name="合計 2" xfId="85"/>
-    <cellStyle name="合計 2 2" xfId="86"/>
-    <cellStyle name="合計 3" xfId="87"/>
-    <cellStyle name="合計 3 2" xfId="88"/>
-    <cellStyle name="好 2" xfId="89"/>
-    <cellStyle name="好 2 2" xfId="90"/>
-    <cellStyle name="好 3" xfId="91"/>
-    <cellStyle name="好 3 2" xfId="92"/>
+    <cellStyle name="千分位[0] 2" xfId="80" xr:uid="{00000000-0005-0000-0000-000050000000}"/>
+    <cellStyle name="中等 2" xfId="81" xr:uid="{00000000-0005-0000-0000-000051000000}"/>
+    <cellStyle name="中等 2 2" xfId="82" xr:uid="{00000000-0005-0000-0000-000052000000}"/>
+    <cellStyle name="中等 3" xfId="83" xr:uid="{00000000-0005-0000-0000-000053000000}"/>
+    <cellStyle name="中等 3 2" xfId="84" xr:uid="{00000000-0005-0000-0000-000054000000}"/>
+    <cellStyle name="合計 2" xfId="85" xr:uid="{00000000-0005-0000-0000-000055000000}"/>
+    <cellStyle name="合計 2 2" xfId="86" xr:uid="{00000000-0005-0000-0000-000056000000}"/>
+    <cellStyle name="合計 3" xfId="87" xr:uid="{00000000-0005-0000-0000-000057000000}"/>
+    <cellStyle name="合計 3 2" xfId="88" xr:uid="{00000000-0005-0000-0000-000058000000}"/>
+    <cellStyle name="好 2" xfId="89" xr:uid="{00000000-0005-0000-0000-000059000000}"/>
+    <cellStyle name="好 2 2" xfId="90" xr:uid="{00000000-0005-0000-0000-00005A000000}"/>
+    <cellStyle name="好 3" xfId="91" xr:uid="{00000000-0005-0000-0000-00005B000000}"/>
+    <cellStyle name="好 3 2" xfId="92" xr:uid="{00000000-0005-0000-0000-00005C000000}"/>
     <cellStyle name="百分比" xfId="93" builtinId="5"/>
-    <cellStyle name="百分比 2" xfId="94"/>
-    <cellStyle name="計算方式 2" xfId="95"/>
-    <cellStyle name="計算方式 2 2" xfId="96"/>
-    <cellStyle name="計算方式 3" xfId="97"/>
-    <cellStyle name="計算方式 3 2" xfId="98"/>
-    <cellStyle name="連結的儲存格 2" xfId="99"/>
-    <cellStyle name="連結的儲存格 2 2" xfId="100"/>
-    <cellStyle name="連結的儲存格 3" xfId="101"/>
-    <cellStyle name="連結的儲存格 3 2" xfId="102"/>
-    <cellStyle name="備註 2" xfId="103"/>
-    <cellStyle name="備註 2 2" xfId="104"/>
-    <cellStyle name="備註 3" xfId="105"/>
-    <cellStyle name="備註 3 2" xfId="106"/>
-    <cellStyle name="說明文字 2" xfId="107"/>
-    <cellStyle name="說明文字 2 2" xfId="108"/>
-    <cellStyle name="說明文字 3" xfId="109"/>
-    <cellStyle name="說明文字 3 2" xfId="110"/>
-    <cellStyle name="輔色1 2" xfId="111"/>
-    <cellStyle name="輔色1 2 2" xfId="112"/>
-    <cellStyle name="輔色1 3" xfId="113"/>
-    <cellStyle name="輔色1 3 2" xfId="114"/>
-    <cellStyle name="輔色2 2" xfId="115"/>
-    <cellStyle name="輔色2 2 2" xfId="116"/>
-    <cellStyle name="輔色2 3" xfId="117"/>
-    <cellStyle name="輔色2 3 2" xfId="118"/>
-    <cellStyle name="輔色3 2" xfId="119"/>
-    <cellStyle name="輔色3 2 2" xfId="120"/>
-    <cellStyle name="輔色3 3" xfId="121"/>
-    <cellStyle name="輔色3 3 2" xfId="122"/>
-    <cellStyle name="輔色4 2" xfId="123"/>
-    <cellStyle name="輔色4 2 2" xfId="124"/>
-    <cellStyle name="輔色4 3" xfId="125"/>
-    <cellStyle name="輔色4 3 2" xfId="126"/>
-    <cellStyle name="輔色5 2" xfId="127"/>
-    <cellStyle name="輔色5 2 2" xfId="128"/>
-    <cellStyle name="輔色5 3" xfId="129"/>
-    <cellStyle name="輔色5 3 2" xfId="130"/>
-    <cellStyle name="輔色6 2" xfId="131"/>
-    <cellStyle name="輔色6 2 2" xfId="132"/>
-    <cellStyle name="輔色6 3" xfId="133"/>
-    <cellStyle name="輔色6 3 2" xfId="134"/>
-    <cellStyle name="標題 1 2" xfId="135"/>
-    <cellStyle name="標題 1 2 2" xfId="136"/>
-    <cellStyle name="標題 1 3" xfId="137"/>
-    <cellStyle name="標題 1 3 2" xfId="138"/>
-    <cellStyle name="標題 2 2" xfId="139"/>
-    <cellStyle name="標題 2 2 2" xfId="140"/>
-    <cellStyle name="標題 2 3" xfId="141"/>
-    <cellStyle name="標題 2 3 2" xfId="142"/>
-    <cellStyle name="標題 3 2" xfId="143"/>
-    <cellStyle name="標題 3 2 2" xfId="144"/>
-    <cellStyle name="標題 3 3" xfId="145"/>
-    <cellStyle name="標題 3 3 2" xfId="146"/>
-    <cellStyle name="標題 4 2" xfId="147"/>
-    <cellStyle name="標題 4 2 2" xfId="148"/>
-    <cellStyle name="標題 4 3" xfId="149"/>
-    <cellStyle name="標題 4 3 2" xfId="150"/>
-    <cellStyle name="標題 5" xfId="151"/>
-    <cellStyle name="標題 5 2" xfId="152"/>
-    <cellStyle name="標題 6" xfId="153"/>
-    <cellStyle name="標題 6 2" xfId="154"/>
-    <cellStyle name="輸入 2" xfId="155"/>
-    <cellStyle name="輸入 2 2" xfId="156"/>
-    <cellStyle name="輸入 3" xfId="157"/>
-    <cellStyle name="輸入 3 2" xfId="158"/>
-    <cellStyle name="輸出 2" xfId="159"/>
-    <cellStyle name="輸出 2 2" xfId="160"/>
-    <cellStyle name="輸出 3" xfId="161"/>
-    <cellStyle name="輸出 3 2" xfId="162"/>
-    <cellStyle name="檢查儲存格 2" xfId="163"/>
-    <cellStyle name="檢查儲存格 2 2" xfId="164"/>
-    <cellStyle name="檢查儲存格 3" xfId="165"/>
-    <cellStyle name="檢查儲存格 3 2" xfId="166"/>
-    <cellStyle name="壞 2" xfId="167"/>
-    <cellStyle name="壞 2 2" xfId="168"/>
-    <cellStyle name="壞 3" xfId="169"/>
-    <cellStyle name="壞 3 2" xfId="170"/>
-    <cellStyle name="警告文字 2" xfId="171"/>
-    <cellStyle name="警告文字 2 2" xfId="172"/>
-    <cellStyle name="警告文字 3" xfId="173"/>
-    <cellStyle name="警告文字 3 2" xfId="174"/>
+    <cellStyle name="百分比 2" xfId="94" xr:uid="{00000000-0005-0000-0000-00005E000000}"/>
+    <cellStyle name="計算方式 2" xfId="95" xr:uid="{00000000-0005-0000-0000-00005F000000}"/>
+    <cellStyle name="計算方式 2 2" xfId="96" xr:uid="{00000000-0005-0000-0000-000060000000}"/>
+    <cellStyle name="計算方式 3" xfId="97" xr:uid="{00000000-0005-0000-0000-000061000000}"/>
+    <cellStyle name="計算方式 3 2" xfId="98" xr:uid="{00000000-0005-0000-0000-000062000000}"/>
+    <cellStyle name="連結的儲存格 2" xfId="99" xr:uid="{00000000-0005-0000-0000-000063000000}"/>
+    <cellStyle name="連結的儲存格 2 2" xfId="100" xr:uid="{00000000-0005-0000-0000-000064000000}"/>
+    <cellStyle name="連結的儲存格 3" xfId="101" xr:uid="{00000000-0005-0000-0000-000065000000}"/>
+    <cellStyle name="連結的儲存格 3 2" xfId="102" xr:uid="{00000000-0005-0000-0000-000066000000}"/>
+    <cellStyle name="備註 2" xfId="103" xr:uid="{00000000-0005-0000-0000-000067000000}"/>
+    <cellStyle name="備註 2 2" xfId="104" xr:uid="{00000000-0005-0000-0000-000068000000}"/>
+    <cellStyle name="備註 3" xfId="105" xr:uid="{00000000-0005-0000-0000-000069000000}"/>
+    <cellStyle name="備註 3 2" xfId="106" xr:uid="{00000000-0005-0000-0000-00006A000000}"/>
+    <cellStyle name="說明文字 2" xfId="107" xr:uid="{00000000-0005-0000-0000-00006B000000}"/>
+    <cellStyle name="說明文字 2 2" xfId="108" xr:uid="{00000000-0005-0000-0000-00006C000000}"/>
+    <cellStyle name="說明文字 3" xfId="109" xr:uid="{00000000-0005-0000-0000-00006D000000}"/>
+    <cellStyle name="說明文字 3 2" xfId="110" xr:uid="{00000000-0005-0000-0000-00006E000000}"/>
+    <cellStyle name="輔色1 2" xfId="111" xr:uid="{00000000-0005-0000-0000-00006F000000}"/>
+    <cellStyle name="輔色1 2 2" xfId="112" xr:uid="{00000000-0005-0000-0000-000070000000}"/>
+    <cellStyle name="輔色1 3" xfId="113" xr:uid="{00000000-0005-0000-0000-000071000000}"/>
+    <cellStyle name="輔色1 3 2" xfId="114" xr:uid="{00000000-0005-0000-0000-000072000000}"/>
+    <cellStyle name="輔色2 2" xfId="115" xr:uid="{00000000-0005-0000-0000-000073000000}"/>
+    <cellStyle name="輔色2 2 2" xfId="116" xr:uid="{00000000-0005-0000-0000-000074000000}"/>
+    <cellStyle name="輔色2 3" xfId="117" xr:uid="{00000000-0005-0000-0000-000075000000}"/>
+    <cellStyle name="輔色2 3 2" xfId="118" xr:uid="{00000000-0005-0000-0000-000076000000}"/>
+    <cellStyle name="輔色3 2" xfId="119" xr:uid="{00000000-0005-0000-0000-000077000000}"/>
+    <cellStyle name="輔色3 2 2" xfId="120" xr:uid="{00000000-0005-0000-0000-000078000000}"/>
+    <cellStyle name="輔色3 3" xfId="121" xr:uid="{00000000-0005-0000-0000-000079000000}"/>
+    <cellStyle name="輔色3 3 2" xfId="122" xr:uid="{00000000-0005-0000-0000-00007A000000}"/>
+    <cellStyle name="輔色4 2" xfId="123" xr:uid="{00000000-0005-0000-0000-00007B000000}"/>
+    <cellStyle name="輔色4 2 2" xfId="124" xr:uid="{00000000-0005-0000-0000-00007C000000}"/>
+    <cellStyle name="輔色4 3" xfId="125" xr:uid="{00000000-0005-0000-0000-00007D000000}"/>
+    <cellStyle name="輔色4 3 2" xfId="126" xr:uid="{00000000-0005-0000-0000-00007E000000}"/>
+    <cellStyle name="輔色5 2" xfId="127" xr:uid="{00000000-0005-0000-0000-00007F000000}"/>
+    <cellStyle name="輔色5 2 2" xfId="128" xr:uid="{00000000-0005-0000-0000-000080000000}"/>
+    <cellStyle name="輔色5 3" xfId="129" xr:uid="{00000000-0005-0000-0000-000081000000}"/>
+    <cellStyle name="輔色5 3 2" xfId="130" xr:uid="{00000000-0005-0000-0000-000082000000}"/>
+    <cellStyle name="輔色6 2" xfId="131" xr:uid="{00000000-0005-0000-0000-000083000000}"/>
+    <cellStyle name="輔色6 2 2" xfId="132" xr:uid="{00000000-0005-0000-0000-000084000000}"/>
+    <cellStyle name="輔色6 3" xfId="133" xr:uid="{00000000-0005-0000-0000-000085000000}"/>
+    <cellStyle name="輔色6 3 2" xfId="134" xr:uid="{00000000-0005-0000-0000-000086000000}"/>
+    <cellStyle name="標題 1 2" xfId="135" xr:uid="{00000000-0005-0000-0000-000087000000}"/>
+    <cellStyle name="標題 1 2 2" xfId="136" xr:uid="{00000000-0005-0000-0000-000088000000}"/>
+    <cellStyle name="標題 1 3" xfId="137" xr:uid="{00000000-0005-0000-0000-000089000000}"/>
+    <cellStyle name="標題 1 3 2" xfId="138" xr:uid="{00000000-0005-0000-0000-00008A000000}"/>
+    <cellStyle name="標題 2 2" xfId="139" xr:uid="{00000000-0005-0000-0000-00008B000000}"/>
+    <cellStyle name="標題 2 2 2" xfId="140" xr:uid="{00000000-0005-0000-0000-00008C000000}"/>
+    <cellStyle name="標題 2 3" xfId="141" xr:uid="{00000000-0005-0000-0000-00008D000000}"/>
+    <cellStyle name="標題 2 3 2" xfId="142" xr:uid="{00000000-0005-0000-0000-00008E000000}"/>
+    <cellStyle name="標題 3 2" xfId="143" xr:uid="{00000000-0005-0000-0000-00008F000000}"/>
+    <cellStyle name="標題 3 2 2" xfId="144" xr:uid="{00000000-0005-0000-0000-000090000000}"/>
+    <cellStyle name="標題 3 3" xfId="145" xr:uid="{00000000-0005-0000-0000-000091000000}"/>
+    <cellStyle name="標題 3 3 2" xfId="146" xr:uid="{00000000-0005-0000-0000-000092000000}"/>
+    <cellStyle name="標題 4 2" xfId="147" xr:uid="{00000000-0005-0000-0000-000093000000}"/>
+    <cellStyle name="標題 4 2 2" xfId="148" xr:uid="{00000000-0005-0000-0000-000094000000}"/>
+    <cellStyle name="標題 4 3" xfId="149" xr:uid="{00000000-0005-0000-0000-000095000000}"/>
+    <cellStyle name="標題 4 3 2" xfId="150" xr:uid="{00000000-0005-0000-0000-000096000000}"/>
+    <cellStyle name="標題 5" xfId="151" xr:uid="{00000000-0005-0000-0000-000097000000}"/>
+    <cellStyle name="標題 5 2" xfId="152" xr:uid="{00000000-0005-0000-0000-000098000000}"/>
+    <cellStyle name="標題 6" xfId="153" xr:uid="{00000000-0005-0000-0000-000099000000}"/>
+    <cellStyle name="標題 6 2" xfId="154" xr:uid="{00000000-0005-0000-0000-00009A000000}"/>
+    <cellStyle name="輸入 2" xfId="155" xr:uid="{00000000-0005-0000-0000-00009B000000}"/>
+    <cellStyle name="輸入 2 2" xfId="156" xr:uid="{00000000-0005-0000-0000-00009C000000}"/>
+    <cellStyle name="輸入 3" xfId="157" xr:uid="{00000000-0005-0000-0000-00009D000000}"/>
+    <cellStyle name="輸入 3 2" xfId="158" xr:uid="{00000000-0005-0000-0000-00009E000000}"/>
+    <cellStyle name="輸出 2" xfId="159" xr:uid="{00000000-0005-0000-0000-00009F000000}"/>
+    <cellStyle name="輸出 2 2" xfId="160" xr:uid="{00000000-0005-0000-0000-0000A0000000}"/>
+    <cellStyle name="輸出 3" xfId="161" xr:uid="{00000000-0005-0000-0000-0000A1000000}"/>
+    <cellStyle name="輸出 3 2" xfId="162" xr:uid="{00000000-0005-0000-0000-0000A2000000}"/>
+    <cellStyle name="檢查儲存格 2" xfId="163" xr:uid="{00000000-0005-0000-0000-0000A3000000}"/>
+    <cellStyle name="檢查儲存格 2 2" xfId="164" xr:uid="{00000000-0005-0000-0000-0000A4000000}"/>
+    <cellStyle name="檢查儲存格 3" xfId="165" xr:uid="{00000000-0005-0000-0000-0000A5000000}"/>
+    <cellStyle name="檢查儲存格 3 2" xfId="166" xr:uid="{00000000-0005-0000-0000-0000A6000000}"/>
+    <cellStyle name="壞 2" xfId="167" xr:uid="{00000000-0005-0000-0000-0000A7000000}"/>
+    <cellStyle name="壞 2 2" xfId="168" xr:uid="{00000000-0005-0000-0000-0000A8000000}"/>
+    <cellStyle name="壞 3" xfId="169" xr:uid="{00000000-0005-0000-0000-0000A9000000}"/>
+    <cellStyle name="壞 3 2" xfId="170" xr:uid="{00000000-0005-0000-0000-0000AA000000}"/>
+    <cellStyle name="警告文字 2" xfId="171" xr:uid="{00000000-0005-0000-0000-0000AB000000}"/>
+    <cellStyle name="警告文字 2 2" xfId="172" xr:uid="{00000000-0005-0000-0000-0000AC000000}"/>
+    <cellStyle name="警告文字 3" xfId="173" xr:uid="{00000000-0005-0000-0000-0000AD000000}"/>
+    <cellStyle name="警告文字 3 2" xfId="174" xr:uid="{00000000-0005-0000-0000-0000AE000000}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
@@ -4324,19 +4281,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/externalLinks/externalLink1.xml><?xml version="1.0" encoding="utf-8"?>
-<externalLink xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" mc:Ignorable="x14">
-  <externalBook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1">
-    <sheetNames>
-      <sheetName val="總表"/>
-    </sheetNames>
-    <sheetDataSet>
-      <sheetData sheetId="0"/>
-    </sheetDataSet>
-  </externalBook>
-</externalLink>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4686,25 +4630,25 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <sheetPr codeName="Sheet1">
     <tabColor indexed="13"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:V50"/>
   <sheetViews>
-    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="13.36328125" defaultRowHeight="31.5" customHeight="1" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.90625" style="10" customWidth="1"/>
-    <col min="2" max="2" width="19.81640625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="25.6328125" style="10" customWidth="1"/>
-    <col min="4" max="4" width="22.81640625" style="10" customWidth="1"/>
-    <col min="5" max="5" width="3.08984375" style="10" customWidth="1"/>
-    <col min="6" max="6" width="30.08984375" style="10" customWidth="1"/>
+    <col min="1" max="1" width="12.90625" style="1" customWidth="1"/>
+    <col min="2" max="2" width="19.81640625" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.6328125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="22.81640625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="3.08984375" style="1" customWidth="1"/>
+    <col min="6" max="6" width="30.08984375" style="1" customWidth="1"/>
     <col min="7" max="7" width="27.453125" style="9" customWidth="1"/>
     <col min="8" max="8" width="27.453125" style="4" customWidth="1"/>
     <col min="9" max="9" width="18.90625" style="9" customWidth="1"/>
@@ -4712,1055 +4656,1051 @@
     <col min="11" max="11" width="20.81640625" style="4" customWidth="1"/>
     <col min="12" max="12" width="24" style="4" customWidth="1"/>
     <col min="13" max="13" width="27.08984375" style="4" customWidth="1"/>
-    <col min="14" max="14" width="6.453125" style="10" customWidth="1"/>
-    <col min="15" max="15" width="24.1796875" style="10" customWidth="1"/>
-    <col min="16" max="16" width="10.1796875" style="10" customWidth="1"/>
-    <col min="17" max="17" width="20.453125" style="37" customWidth="1"/>
-    <col min="18" max="18" width="8.81640625" style="37" customWidth="1"/>
-    <col min="19" max="19" width="21" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="19.36328125" style="10" customWidth="1"/>
-    <col min="21" max="16384" width="13.36328125" style="10"/>
+    <col min="14" max="14" width="6.453125" style="1" customWidth="1"/>
+    <col min="15" max="15" width="24.1796875" style="1" customWidth="1"/>
+    <col min="16" max="16" width="10.1796875" style="1" customWidth="1"/>
+    <col min="17" max="17" width="20.453125" style="34" customWidth="1"/>
+    <col min="18" max="18" width="8.81640625" style="34" customWidth="1"/>
+    <col min="19" max="19" width="21" style="1" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="19.36328125" style="1" customWidth="1"/>
+    <col min="21" max="16384" width="13.36328125" style="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="39.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A1" s="103" t="s">
+      <c r="A1" s="94" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="104"/>
-      <c r="C1" s="104"/>
-      <c r="D1" s="104"/>
-      <c r="E1" s="104"/>
-      <c r="F1" s="105"/>
-      <c r="G1" s="106"/>
-      <c r="H1" s="107"/>
-      <c r="I1" s="106"/>
-      <c r="J1" s="107"/>
-      <c r="K1" s="107"/>
-      <c r="L1" s="107"/>
-      <c r="M1" s="71" t="s">
+      <c r="B1" s="95"/>
+      <c r="C1" s="95"/>
+      <c r="D1" s="95"/>
+      <c r="E1" s="95"/>
+      <c r="F1" s="96"/>
+      <c r="G1" s="97"/>
+      <c r="H1" s="98"/>
+      <c r="I1" s="97"/>
+      <c r="J1" s="98"/>
+      <c r="K1" s="98"/>
+      <c r="L1" s="98"/>
+      <c r="M1" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="N1" s="27"/>
-      <c r="O1" s="12"/>
-      <c r="P1" s="12"/>
-      <c r="Q1" s="36"/>
-      <c r="R1" s="36"/>
+      <c r="N1" s="25"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
     </row>
-    <row r="2" spans="1:22" s="26" customFormat="1" ht="23.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="225" t="s">
+    <row r="2" spans="1:22" s="24" customFormat="1" ht="23.15" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="203" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="226"/>
-      <c r="C2" s="229" t="s">
+      <c r="B2" s="204"/>
+      <c r="C2" s="257" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="231" t="s">
+      <c r="D2" s="259" t="s">
         <v>63</v>
       </c>
-      <c r="E2" s="226"/>
-      <c r="F2" s="254" t="s">
+      <c r="E2" s="204"/>
+      <c r="F2" s="231" t="s">
         <v>27</v>
       </c>
-      <c r="G2" s="256" t="s">
+      <c r="G2" s="233" t="s">
         <v>64</v>
       </c>
-      <c r="H2" s="257"/>
-      <c r="I2" s="266" t="s">
+      <c r="H2" s="234"/>
+      <c r="I2" s="243" t="s">
         <v>41</v>
       </c>
-      <c r="J2" s="267"/>
-      <c r="K2" s="267"/>
-      <c r="L2" s="267"/>
-      <c r="M2" s="268"/>
-      <c r="N2" s="12"/>
-      <c r="O2" s="108"/>
-      <c r="P2" s="36"/>
-      <c r="Q2" s="38"/>
+      <c r="J2" s="244"/>
+      <c r="K2" s="244"/>
+      <c r="L2" s="244"/>
+      <c r="M2" s="245"/>
+      <c r="N2" s="10"/>
+      <c r="O2" s="99"/>
+      <c r="P2" s="34"/>
+      <c r="Q2" s="35"/>
     </row>
-    <row r="3" spans="1:22" s="26" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A3" s="227"/>
-      <c r="B3" s="228"/>
-      <c r="C3" s="230"/>
-      <c r="D3" s="232"/>
-      <c r="E3" s="228"/>
-      <c r="F3" s="255"/>
-      <c r="G3" s="258"/>
-      <c r="H3" s="259"/>
-      <c r="I3" s="30" t="s">
+    <row r="3" spans="1:22" s="24" customFormat="1" ht="23.15" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A3" s="205"/>
+      <c r="B3" s="206"/>
+      <c r="C3" s="258"/>
+      <c r="D3" s="260"/>
+      <c r="E3" s="206"/>
+      <c r="F3" s="232"/>
+      <c r="G3" s="235"/>
+      <c r="H3" s="236"/>
+      <c r="I3" s="28" t="s">
         <v>28</v>
       </c>
-      <c r="J3" s="262" t="s">
+      <c r="J3" s="239" t="s">
         <v>2</v>
       </c>
-      <c r="K3" s="263"/>
-      <c r="L3" s="100" t="s">
+      <c r="K3" s="240"/>
+      <c r="L3" s="91" t="s">
         <v>65</v>
       </c>
-      <c r="M3" s="31" t="s">
+      <c r="M3" s="29" t="s">
         <v>1</v>
       </c>
-      <c r="N3" s="69"/>
-      <c r="O3" s="70"/>
-      <c r="P3" s="75"/>
-      <c r="Q3" s="58"/>
+      <c r="N3" s="64"/>
+      <c r="O3" s="65"/>
+      <c r="P3" s="54"/>
+      <c r="Q3" s="54"/>
     </row>
     <row r="4" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A4" s="239" t="s">
+      <c r="A4" s="268" t="s">
         <v>17</v>
       </c>
-      <c r="B4" s="241" t="s">
+      <c r="B4" s="270" t="s">
         <v>18</v>
       </c>
-      <c r="C4" s="109"/>
-      <c r="D4" s="218"/>
-      <c r="E4" s="219"/>
-      <c r="F4" s="110">
+      <c r="C4" s="100"/>
+      <c r="D4" s="248"/>
+      <c r="E4" s="249"/>
+      <c r="F4" s="101">
         <f>SUM(C4:E4)</f>
         <v>0</v>
       </c>
-      <c r="G4" s="233" t="s">
+      <c r="G4" s="261" t="s">
         <v>25</v>
       </c>
-      <c r="H4" s="234"/>
-      <c r="I4" s="111">
+      <c r="H4" s="262"/>
+      <c r="I4" s="102">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J4" s="201">
+      <c r="J4" s="219">
         <f>C4*I4</f>
         <v>0</v>
       </c>
-      <c r="K4" s="202"/>
-      <c r="L4" s="112">
+      <c r="K4" s="220"/>
+      <c r="L4" s="103">
         <f>D4*I4</f>
         <v>0</v>
       </c>
-      <c r="M4" s="113">
+      <c r="M4" s="104">
         <f>SUM(J4:L4)</f>
         <v>0</v>
       </c>
-      <c r="N4" s="114"/>
-      <c r="O4" s="115"/>
-      <c r="P4" s="76"/>
-      <c r="Q4" s="38"/>
-      <c r="R4" s="10"/>
-      <c r="T4" s="68"/>
+      <c r="N4" s="105"/>
+      <c r="O4" s="106"/>
+      <c r="P4" s="70"/>
+      <c r="Q4" s="35"/>
+      <c r="R4" s="1"/>
+      <c r="T4" s="63"/>
     </row>
     <row r="5" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A5" s="240"/>
-      <c r="B5" s="242"/>
-      <c r="C5" s="109"/>
-      <c r="D5" s="237"/>
-      <c r="E5" s="238"/>
-      <c r="F5" s="110">
+      <c r="A5" s="269"/>
+      <c r="B5" s="271"/>
+      <c r="C5" s="100"/>
+      <c r="D5" s="265"/>
+      <c r="E5" s="266"/>
+      <c r="F5" s="101">
         <f t="shared" ref="F5:F11" si="0">SUM(C5:E5)</f>
         <v>0</v>
       </c>
-      <c r="G5" s="234" t="s">
+      <c r="G5" s="262" t="s">
         <v>44</v>
       </c>
-      <c r="H5" s="243"/>
-      <c r="I5" s="111">
+      <c r="H5" s="272"/>
+      <c r="I5" s="102">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="J5" s="201">
+      <c r="J5" s="219">
         <f t="shared" ref="J5:J9" si="1">C5*I5</f>
         <v>0</v>
       </c>
-      <c r="K5" s="202"/>
-      <c r="L5" s="112">
+      <c r="K5" s="220"/>
+      <c r="L5" s="103">
         <f t="shared" ref="L5:L11" si="2">D5*I5</f>
         <v>0</v>
       </c>
-      <c r="M5" s="113">
+      <c r="M5" s="104">
         <f t="shared" ref="M5:M11" si="3">SUM(J5:L5)</f>
         <v>0</v>
       </c>
-      <c r="N5" s="116"/>
-      <c r="O5" s="115"/>
-      <c r="P5" s="76"/>
-      <c r="Q5" s="38"/>
-      <c r="R5" s="10"/>
-      <c r="T5" s="68"/>
+      <c r="N5" s="107"/>
+      <c r="O5" s="106"/>
+      <c r="P5" s="70"/>
+      <c r="Q5" s="35"/>
+      <c r="R5" s="1"/>
+      <c r="T5" s="63"/>
     </row>
     <row r="6" spans="1:22" ht="46.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A6" s="235" t="s">
+      <c r="A6" s="216" t="s">
         <v>19</v>
       </c>
-      <c r="B6" s="203" t="s">
+      <c r="B6" s="207" t="s">
         <v>20</v>
       </c>
-      <c r="C6" s="109"/>
-      <c r="D6" s="218"/>
-      <c r="E6" s="219"/>
-      <c r="F6" s="110">
+      <c r="C6" s="100"/>
+      <c r="D6" s="248"/>
+      <c r="E6" s="249"/>
+      <c r="F6" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G6" s="215" t="s">
+      <c r="G6" s="263" t="s">
         <v>54</v>
       </c>
-      <c r="H6" s="236"/>
-      <c r="I6" s="111">
+      <c r="H6" s="264"/>
+      <c r="I6" s="102">
         <v>0.02</v>
       </c>
-      <c r="J6" s="201">
+      <c r="J6" s="219">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K6" s="202"/>
-      <c r="L6" s="112">
+      <c r="K6" s="220"/>
+      <c r="L6" s="103">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M6" s="113">
+      <c r="M6" s="104">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N6" s="116"/>
-      <c r="O6" s="115"/>
-      <c r="P6" s="76"/>
-      <c r="Q6" s="33"/>
-      <c r="R6" s="11"/>
-      <c r="T6" s="68"/>
+      <c r="N6" s="107"/>
+      <c r="O6" s="106"/>
+      <c r="P6" s="70"/>
+      <c r="Q6" s="31"/>
+      <c r="R6" s="5"/>
+      <c r="T6" s="63"/>
     </row>
     <row r="7" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A7" s="235"/>
-      <c r="B7" s="203"/>
-      <c r="C7" s="117"/>
-      <c r="D7" s="269"/>
-      <c r="E7" s="270"/>
-      <c r="F7" s="110">
+      <c r="A7" s="216"/>
+      <c r="B7" s="207"/>
+      <c r="C7" s="108"/>
+      <c r="D7" s="246"/>
+      <c r="E7" s="247"/>
+      <c r="F7" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G7" s="214" t="s">
+      <c r="G7" s="267" t="s">
         <v>55</v>
       </c>
-      <c r="H7" s="215"/>
-      <c r="I7" s="111">
+      <c r="H7" s="263"/>
+      <c r="I7" s="102">
         <v>0.02</v>
       </c>
-      <c r="J7" s="201">
+      <c r="J7" s="219">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K7" s="202"/>
-      <c r="L7" s="112">
+      <c r="K7" s="220"/>
+      <c r="L7" s="103">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M7" s="113">
+      <c r="M7" s="104">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N7" s="114"/>
-      <c r="O7" s="115"/>
-      <c r="P7" s="76"/>
-      <c r="Q7" s="33"/>
-      <c r="R7" s="11"/>
-      <c r="T7" s="68"/>
+      <c r="N7" s="105"/>
+      <c r="O7" s="106"/>
+      <c r="P7" s="70"/>
+      <c r="Q7" s="31"/>
+      <c r="R7" s="5"/>
+      <c r="T7" s="63"/>
     </row>
     <row r="8" spans="1:22" ht="39.75" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A8" s="235"/>
-      <c r="B8" s="203"/>
-      <c r="C8" s="109"/>
-      <c r="D8" s="218"/>
-      <c r="E8" s="219"/>
-      <c r="F8" s="110">
+      <c r="A8" s="216"/>
+      <c r="B8" s="207"/>
+      <c r="C8" s="100"/>
+      <c r="D8" s="248"/>
+      <c r="E8" s="249"/>
+      <c r="F8" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G8" s="212" t="s">
+      <c r="G8" s="267" t="s">
         <v>56</v>
       </c>
-      <c r="H8" s="213"/>
-      <c r="I8" s="111">
+      <c r="H8" s="263"/>
+      <c r="I8" s="102">
         <v>0.02</v>
       </c>
-      <c r="J8" s="201">
+      <c r="J8" s="219">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="202"/>
-      <c r="L8" s="112">
+      <c r="K8" s="220"/>
+      <c r="L8" s="103">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M8" s="113">
+      <c r="M8" s="104">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N8" s="114"/>
-      <c r="O8" s="115"/>
-      <c r="P8" s="76"/>
-      <c r="Q8" s="33"/>
-      <c r="R8" s="11"/>
-      <c r="T8" s="68"/>
+      <c r="N8" s="105"/>
+      <c r="O8" s="106"/>
+      <c r="P8" s="70"/>
+      <c r="Q8" s="31"/>
+      <c r="R8" s="5"/>
+      <c r="T8" s="63"/>
     </row>
     <row r="9" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A9" s="101" t="s">
+      <c r="A9" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="B9" s="99" t="s">
+      <c r="B9" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="109"/>
-      <c r="D9" s="210"/>
-      <c r="E9" s="211"/>
-      <c r="F9" s="110">
+      <c r="C9" s="100"/>
+      <c r="D9" s="255"/>
+      <c r="E9" s="256"/>
+      <c r="F9" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G9" s="212" t="s">
+      <c r="G9" s="267" t="s">
         <v>57</v>
       </c>
-      <c r="H9" s="213"/>
-      <c r="I9" s="118">
+      <c r="H9" s="263"/>
+      <c r="I9" s="109">
         <v>0.1</v>
       </c>
-      <c r="J9" s="201">
+      <c r="J9" s="219">
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K9" s="202"/>
-      <c r="L9" s="112">
+      <c r="K9" s="220"/>
+      <c r="L9" s="103">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M9" s="113">
+      <c r="M9" s="104">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N9" s="114"/>
-      <c r="O9" s="119"/>
-      <c r="P9" s="76"/>
-      <c r="Q9" s="33"/>
-      <c r="R9" s="11"/>
-      <c r="T9" s="68"/>
+      <c r="N9" s="105"/>
+      <c r="O9" s="110"/>
+      <c r="P9" s="70"/>
+      <c r="Q9" s="31"/>
+      <c r="R9" s="5"/>
+      <c r="T9" s="63"/>
     </row>
     <row r="10" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A10" s="101" t="s">
+      <c r="A10" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="B10" s="99" t="s">
+      <c r="B10" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="120"/>
-      <c r="D10" s="210"/>
-      <c r="E10" s="211"/>
-      <c r="F10" s="110">
+      <c r="C10" s="111"/>
+      <c r="D10" s="255"/>
+      <c r="E10" s="256"/>
+      <c r="F10" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G10" s="212" t="s">
+      <c r="G10" s="267" t="s">
         <v>58</v>
       </c>
-      <c r="H10" s="213"/>
-      <c r="I10" s="118">
+      <c r="H10" s="263"/>
+      <c r="I10" s="109">
         <v>0.5</v>
       </c>
-      <c r="J10" s="201">
+      <c r="J10" s="219">
         <f>C10*I10</f>
         <v>0</v>
       </c>
-      <c r="K10" s="202"/>
-      <c r="L10" s="112">
+      <c r="K10" s="220"/>
+      <c r="L10" s="103">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M10" s="113">
+      <c r="M10" s="104">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N10" s="114"/>
-      <c r="O10" s="119"/>
-      <c r="P10" s="76"/>
-      <c r="Q10" s="33"/>
-      <c r="R10" s="11"/>
+      <c r="N10" s="105"/>
+      <c r="O10" s="110"/>
+      <c r="P10" s="70"/>
+      <c r="Q10" s="31"/>
+      <c r="R10" s="5"/>
     </row>
     <row r="11" spans="1:22" ht="66.900000000000006" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A11" s="101" t="s">
+      <c r="A11" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="B11" s="99" t="s">
+      <c r="B11" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="C11" s="109"/>
-      <c r="D11" s="271"/>
-      <c r="E11" s="272"/>
-      <c r="F11" s="110">
+      <c r="C11" s="100"/>
+      <c r="D11" s="250"/>
+      <c r="E11" s="251"/>
+      <c r="F11" s="101">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="G11" s="212" t="s">
+      <c r="G11" s="267" t="s">
         <v>59</v>
       </c>
-      <c r="H11" s="213"/>
-      <c r="I11" s="121">
+      <c r="H11" s="263"/>
+      <c r="I11" s="112">
         <v>1</v>
       </c>
-      <c r="J11" s="201">
+      <c r="J11" s="219">
         <f t="shared" ref="J11" si="4">C11*I11</f>
         <v>0</v>
       </c>
-      <c r="K11" s="202"/>
-      <c r="L11" s="112">
+      <c r="K11" s="220"/>
+      <c r="L11" s="103">
         <f t="shared" si="2"/>
         <v>0</v>
       </c>
-      <c r="M11" s="113">
+      <c r="M11" s="104">
         <f t="shared" si="3"/>
         <v>0</v>
       </c>
-      <c r="N11" s="114"/>
-      <c r="O11" s="119"/>
-      <c r="P11" s="76"/>
-      <c r="Q11" s="33"/>
-      <c r="R11" s="11"/>
+      <c r="N11" s="105"/>
+      <c r="O11" s="110"/>
+      <c r="P11" s="70"/>
+      <c r="Q11" s="31"/>
+      <c r="R11" s="5"/>
     </row>
     <row r="12" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A12" s="287" t="s">
+      <c r="A12" s="211" t="s">
         <v>74</v>
       </c>
-      <c r="B12" s="277"/>
-      <c r="C12" s="109"/>
-      <c r="D12" s="276"/>
-      <c r="E12" s="277"/>
-      <c r="F12" s="122">
-        <v>0</v>
-      </c>
-      <c r="G12" s="278"/>
-      <c r="H12" s="279"/>
-      <c r="I12" s="111">
+      <c r="B12" s="198"/>
+      <c r="C12" s="100"/>
+      <c r="D12" s="197"/>
+      <c r="E12" s="198"/>
+      <c r="F12" s="113">
+        <v>0</v>
+      </c>
+      <c r="G12" s="199"/>
+      <c r="H12" s="200"/>
+      <c r="I12" s="102">
         <v>5.0000000000000001E-3</v>
       </c>
-      <c r="J12" s="201"/>
-      <c r="K12" s="202"/>
-      <c r="L12" s="123"/>
-      <c r="M12" s="124">
+      <c r="J12" s="219"/>
+      <c r="K12" s="220"/>
+      <c r="L12" s="114"/>
+      <c r="M12" s="115">
         <f>F12*I12</f>
         <v>0</v>
       </c>
-      <c r="N12" s="114"/>
-      <c r="O12" s="119"/>
-      <c r="P12" s="84"/>
-      <c r="Q12" s="38"/>
-      <c r="R12" s="10"/>
+      <c r="N12" s="105"/>
+      <c r="O12" s="110"/>
+      <c r="P12" s="34"/>
+      <c r="Q12" s="35"/>
+      <c r="R12" s="1"/>
     </row>
     <row r="13" spans="1:22" ht="39.9" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A13" s="287" t="s">
+      <c r="A13" s="211" t="s">
         <v>73</v>
       </c>
-      <c r="B13" s="277"/>
-      <c r="C13" s="109"/>
-      <c r="D13" s="276"/>
-      <c r="E13" s="277"/>
-      <c r="F13" s="122">
-        <v>0</v>
-      </c>
-      <c r="G13" s="278"/>
-      <c r="H13" s="279"/>
-      <c r="I13" s="111">
+      <c r="B13" s="198"/>
+      <c r="C13" s="100"/>
+      <c r="D13" s="197"/>
+      <c r="E13" s="198"/>
+      <c r="F13" s="113">
+        <v>0</v>
+      </c>
+      <c r="G13" s="199"/>
+      <c r="H13" s="200"/>
+      <c r="I13" s="102">
         <v>0.02</v>
       </c>
-      <c r="J13" s="201"/>
-      <c r="K13" s="202"/>
-      <c r="L13" s="123"/>
-      <c r="M13" s="124">
+      <c r="J13" s="219"/>
+      <c r="K13" s="220"/>
+      <c r="L13" s="114"/>
+      <c r="M13" s="115">
         <f>F13*I13</f>
         <v>0</v>
       </c>
-      <c r="N13" s="114"/>
-      <c r="O13" s="119"/>
-      <c r="P13" s="84"/>
-      <c r="Q13" s="38"/>
-      <c r="R13" s="10"/>
+      <c r="N13" s="105"/>
+      <c r="O13" s="110"/>
+      <c r="P13" s="34"/>
+      <c r="Q13" s="35"/>
+      <c r="R13" s="1"/>
     </row>
     <row r="14" spans="1:22" ht="50.15" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A14" s="216" t="s">
+      <c r="A14" s="212" t="s">
         <v>69</v>
       </c>
-      <c r="B14" s="217"/>
-      <c r="C14" s="125">
+      <c r="B14" s="213"/>
+      <c r="C14" s="116">
         <f>SUM(C4:C11)</f>
         <v>0</v>
       </c>
-      <c r="D14" s="260">
+      <c r="D14" s="237">
         <f>SUM(D4:E11)</f>
         <v>0</v>
       </c>
-      <c r="E14" s="261"/>
-      <c r="F14" s="126">
-        <f>SUM(F4:F12)</f>
-        <v>0</v>
-      </c>
-      <c r="G14" s="223"/>
-      <c r="H14" s="224"/>
-      <c r="I14" s="127"/>
-      <c r="J14" s="264">
+      <c r="E14" s="238"/>
+      <c r="F14" s="117">
+        <f>SUM(F4:F13)</f>
+        <v>0</v>
+      </c>
+      <c r="G14" s="282"/>
+      <c r="H14" s="283"/>
+      <c r="I14" s="118"/>
+      <c r="J14" s="241">
         <f>SUM(J4:K13)</f>
         <v>0</v>
       </c>
-      <c r="K14" s="265"/>
-      <c r="L14" s="128">
+      <c r="K14" s="242"/>
+      <c r="L14" s="119">
         <f>SUM(L4:L13)</f>
         <v>0</v>
       </c>
-      <c r="M14" s="129">
+      <c r="M14" s="120">
         <f>SUM(M4:M13)</f>
         <v>0</v>
       </c>
-      <c r="N14" s="114"/>
-      <c r="O14" s="130"/>
-      <c r="P14" s="85"/>
-      <c r="Q14" s="83"/>
-      <c r="R14" s="10"/>
+      <c r="N14" s="105"/>
+      <c r="O14" s="121"/>
+      <c r="P14" s="78"/>
+      <c r="Q14" s="77"/>
+      <c r="R14" s="1"/>
     </row>
-    <row r="15" spans="1:22" s="59" customFormat="1" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A15" s="131"/>
-      <c r="B15" s="132"/>
-      <c r="C15" s="133">
-        <v>0</v>
-      </c>
-      <c r="D15" s="134">
-        <v>0</v>
-      </c>
-      <c r="E15" s="135"/>
-      <c r="F15" s="135">
-        <v>0</v>
-      </c>
-      <c r="G15" s="136"/>
-      <c r="H15" s="137">
-        <v>0</v>
-      </c>
-      <c r="I15" s="284" t="s">
+    <row r="15" spans="1:22" s="55" customFormat="1" ht="25.5" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
+      <c r="A15" s="122"/>
+      <c r="B15" s="123"/>
+      <c r="C15" s="124">
+        <v>0</v>
+      </c>
+      <c r="D15" s="125">
+        <v>0</v>
+      </c>
+      <c r="E15" s="126"/>
+      <c r="F15" s="126">
+        <v>0</v>
+      </c>
+      <c r="G15" s="127"/>
+      <c r="H15" s="128">
+        <v>0</v>
+      </c>
+      <c r="I15" s="208" t="s">
         <v>72</v>
       </c>
-      <c r="J15" s="285"/>
-      <c r="K15" s="286"/>
-      <c r="L15" s="138"/>
-      <c r="M15" s="139">
+      <c r="J15" s="209"/>
+      <c r="K15" s="210"/>
+      <c r="L15" s="129"/>
+      <c r="M15" s="130">
         <f>L15*2%</f>
         <v>0</v>
       </c>
-      <c r="N15" s="140"/>
-      <c r="O15" s="140">
+      <c r="N15" s="131"/>
+      <c r="O15" s="131">
         <v>0.02</v>
       </c>
-      <c r="P15" s="60"/>
-      <c r="Q15" s="61"/>
+      <c r="Q15" s="56"/>
     </row>
     <row r="16" spans="1:22" ht="30" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A16" s="225" t="s">
+      <c r="A16" s="203" t="s">
         <v>62</v>
       </c>
-      <c r="B16" s="226"/>
-      <c r="C16" s="290" t="s">
+      <c r="B16" s="204"/>
+      <c r="C16" s="217" t="s">
         <v>66</v>
       </c>
-      <c r="D16" s="288" t="s">
+      <c r="D16" s="214" t="s">
         <v>29</v>
       </c>
-      <c r="E16" s="46"/>
-      <c r="F16" s="32" t="s">
+      <c r="E16" s="42"/>
+      <c r="F16" s="30" t="s">
         <v>26</v>
       </c>
-      <c r="G16" s="19" t="s">
+      <c r="G16" s="17" t="s">
         <v>11</v>
       </c>
-      <c r="H16" s="20" t="s">
+      <c r="H16" s="18" t="s">
         <v>5</v>
       </c>
-      <c r="I16" s="55" t="s">
+      <c r="I16" s="51" t="s">
         <v>6</v>
       </c>
-      <c r="J16" s="54"/>
-      <c r="K16" s="141"/>
-      <c r="L16" s="141"/>
-      <c r="M16" s="142"/>
-      <c r="N16" s="143">
+      <c r="J16" s="50"/>
+      <c r="K16" s="132"/>
+      <c r="L16" s="132"/>
+      <c r="M16" s="133"/>
+      <c r="N16" s="134">
         <v>1029271555.715</v>
       </c>
-      <c r="O16" s="130"/>
-      <c r="P16" s="37"/>
-      <c r="Q16" s="35"/>
-      <c r="R16" s="10"/>
-      <c r="V16" s="13"/>
+      <c r="O16" s="121"/>
+      <c r="P16" s="34"/>
+      <c r="Q16" s="33"/>
+      <c r="R16" s="1"/>
+      <c r="V16" s="11"/>
     </row>
     <row r="17" spans="1:22" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A17" s="227"/>
-      <c r="B17" s="228"/>
-      <c r="C17" s="291"/>
-      <c r="D17" s="289"/>
-      <c r="E17" s="46"/>
-      <c r="F17" s="51" t="s">
+      <c r="A17" s="205"/>
+      <c r="B17" s="206"/>
+      <c r="C17" s="218"/>
+      <c r="D17" s="215"/>
+      <c r="E17" s="42"/>
+      <c r="F17" s="47" t="s">
         <v>67</v>
       </c>
-      <c r="G17" s="144"/>
-      <c r="H17" s="144"/>
-      <c r="I17" s="145"/>
-      <c r="J17" s="54"/>
-      <c r="K17" s="249" t="s">
+      <c r="G17" s="135"/>
+      <c r="H17" s="135"/>
+      <c r="I17" s="136"/>
+      <c r="J17" s="50"/>
+      <c r="K17" s="226" t="s">
         <v>46</v>
       </c>
-      <c r="L17" s="250"/>
-      <c r="M17" s="146">
+      <c r="L17" s="227"/>
+      <c r="M17" s="137">
         <f>M14+M15</f>
         <v>0</v>
       </c>
-      <c r="N17" s="147" t="s">
+      <c r="N17" s="138" t="s">
         <v>42</v>
       </c>
-      <c r="O17" s="130" t="s">
+      <c r="O17" s="121" t="s">
         <v>37</v>
       </c>
-      <c r="P17" s="37"/>
-      <c r="Q17" s="35"/>
-      <c r="R17" s="10"/>
-      <c r="V17" s="17"/>
+      <c r="P17" s="34"/>
+      <c r="Q17" s="33"/>
+      <c r="R17" s="1"/>
+      <c r="V17" s="15"/>
     </row>
     <row r="18" spans="1:22" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A18" s="101" t="s">
+      <c r="A18" s="92" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="99" t="s">
+      <c r="B18" s="90" t="s">
         <v>18</v>
       </c>
-      <c r="C18" s="148"/>
-      <c r="D18" s="149">
+      <c r="C18" s="139"/>
+      <c r="D18" s="140">
         <f>F4+F5-C18</f>
         <v>0</v>
       </c>
-      <c r="E18" s="150"/>
-      <c r="F18" s="51" t="s">
+      <c r="E18" s="141"/>
+      <c r="F18" s="47" t="s">
         <v>68</v>
       </c>
-      <c r="G18" s="144"/>
-      <c r="H18" s="144"/>
-      <c r="I18" s="145"/>
-      <c r="J18" s="54"/>
-      <c r="K18" s="282" t="s">
+      <c r="G18" s="135"/>
+      <c r="H18" s="135"/>
+      <c r="I18" s="136"/>
+      <c r="J18" s="50"/>
+      <c r="K18" s="188" t="s">
         <v>47</v>
       </c>
-      <c r="L18" s="283"/>
-      <c r="M18" s="151">
+      <c r="L18" s="189"/>
+      <c r="M18" s="142">
         <f>(F14+L15)*1%</f>
         <v>0</v>
       </c>
-      <c r="N18" s="152"/>
-      <c r="O18" s="153">
+      <c r="N18" s="143"/>
+      <c r="O18" s="144">
         <v>0.01</v>
       </c>
-      <c r="P18" s="37"/>
-      <c r="Q18" s="35"/>
-      <c r="R18" s="10"/>
+      <c r="P18" s="34"/>
+      <c r="Q18" s="33"/>
+      <c r="R18" s="1"/>
     </row>
     <row r="19" spans="1:22" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A19" s="235" t="s">
+      <c r="A19" s="216" t="s">
         <v>19</v>
       </c>
-      <c r="B19" s="203" t="s">
+      <c r="B19" s="207" t="s">
         <v>20</v>
       </c>
-      <c r="C19" s="148"/>
-      <c r="D19" s="149">
+      <c r="C19" s="139"/>
+      <c r="D19" s="140">
         <f t="shared" ref="D19:D25" si="5">F6-C19</f>
         <v>0</v>
       </c>
-      <c r="E19" s="154" t="s">
+      <c r="E19" s="145" t="s">
         <v>53</v>
       </c>
-      <c r="F19" s="51" t="s">
+      <c r="F19" s="47" t="s">
         <v>70</v>
       </c>
-      <c r="G19" s="144"/>
-      <c r="H19" s="144"/>
-      <c r="I19" s="145"/>
-      <c r="J19" s="54"/>
-      <c r="K19" s="282" t="s">
+      <c r="G19" s="135"/>
+      <c r="H19" s="135"/>
+      <c r="I19" s="136"/>
+      <c r="J19" s="50"/>
+      <c r="K19" s="188" t="s">
         <v>48</v>
       </c>
-      <c r="L19" s="283"/>
-      <c r="M19" s="151">
+      <c r="L19" s="189"/>
+      <c r="M19" s="142">
         <f>F11</f>
         <v>0</v>
       </c>
-      <c r="N19" s="141"/>
-      <c r="O19" s="155"/>
-      <c r="P19" s="37"/>
-      <c r="Q19" s="35"/>
-      <c r="R19" s="10"/>
+      <c r="N19" s="132"/>
+      <c r="O19" s="146"/>
+      <c r="P19" s="34"/>
+      <c r="Q19" s="33"/>
+      <c r="R19" s="1"/>
     </row>
     <row r="20" spans="1:22" ht="21.9" customHeight="1" x14ac:dyDescent="0.45">
-      <c r="A20" s="235"/>
-      <c r="B20" s="203"/>
-      <c r="C20" s="148"/>
-      <c r="D20" s="149">
+      <c r="A20" s="216"/>
+      <c r="B20" s="207"/>
+      <c r="C20" s="139"/>
+      <c r="D20" s="140">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E20" s="154"/>
-      <c r="F20" s="52" t="s">
-        <v>0</v>
-      </c>
-      <c r="G20" s="156">
+      <c r="E20" s="145"/>
+      <c r="F20" s="48" t="s">
+        <v>0</v>
+      </c>
+      <c r="G20" s="147">
         <f>SUM(G17:G19)</f>
         <v>0</v>
       </c>
-      <c r="H20" s="156">
+      <c r="H20" s="147">
         <f>SUM(H17:H19)</f>
         <v>0</v>
       </c>
-      <c r="I20" s="156">
+      <c r="I20" s="147">
         <f>SUM(I17:I19)</f>
         <v>0</v>
       </c>
-      <c r="J20" s="54"/>
-      <c r="K20" s="107"/>
-      <c r="L20" s="107"/>
-      <c r="M20" s="107"/>
-      <c r="N20" s="155"/>
-      <c r="O20" s="155"/>
-      <c r="P20" s="37"/>
-      <c r="Q20" s="35"/>
-      <c r="R20" s="10"/>
+      <c r="J20" s="50"/>
+      <c r="K20" s="98"/>
+      <c r="L20" s="98"/>
+      <c r="M20" s="98"/>
+      <c r="N20" s="146"/>
+      <c r="O20" s="146"/>
+      <c r="P20" s="34"/>
+      <c r="Q20" s="33"/>
+      <c r="R20" s="1"/>
     </row>
     <row r="21" spans="1:22" ht="21.9" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="A21" s="235"/>
-      <c r="B21" s="203"/>
-      <c r="C21" s="148"/>
-      <c r="D21" s="149">
+      <c r="A21" s="216"/>
+      <c r="B21" s="207"/>
+      <c r="C21" s="139"/>
+      <c r="D21" s="140">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E21" s="154"/>
-      <c r="F21" s="53" t="s">
+      <c r="E21" s="145"/>
+      <c r="F21" s="49" t="s">
         <v>12</v>
       </c>
-      <c r="G21" s="298">
+      <c r="G21" s="194">
         <f>SUM(G20:I20)</f>
         <v>0</v>
       </c>
-      <c r="H21" s="299"/>
-      <c r="I21" s="300"/>
-      <c r="J21" s="54"/>
-      <c r="K21" s="107"/>
-      <c r="L21" s="107"/>
-      <c r="M21" s="107"/>
-      <c r="N21" s="155"/>
-      <c r="O21" s="157"/>
-      <c r="P21" s="86"/>
-      <c r="Q21" s="35"/>
-      <c r="R21" s="10"/>
+      <c r="H21" s="195"/>
+      <c r="I21" s="196"/>
+      <c r="J21" s="50"/>
+      <c r="K21" s="98"/>
+      <c r="L21" s="98"/>
+      <c r="M21" s="98"/>
+      <c r="N21" s="146"/>
+      <c r="O21" s="148"/>
+      <c r="P21" s="34"/>
+      <c r="Q21" s="33"/>
+      <c r="R21" s="1"/>
     </row>
     <row r="22" spans="1:22" ht="29.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A22" s="101" t="s">
+      <c r="A22" s="92" t="s">
         <v>21</v>
       </c>
-      <c r="B22" s="99" t="s">
+      <c r="B22" s="90" t="s">
         <v>22</v>
       </c>
-      <c r="C22" s="148"/>
-      <c r="D22" s="149">
+      <c r="C22" s="139"/>
+      <c r="D22" s="140">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E22" s="158" t="s">
+      <c r="E22" s="149" t="s">
         <v>53</v>
       </c>
-      <c r="F22" s="155"/>
-      <c r="G22" s="107"/>
-      <c r="H22" s="159"/>
-      <c r="I22" s="160">
-        <v>0</v>
-      </c>
-      <c r="J22" s="159"/>
-      <c r="K22" s="159"/>
-      <c r="L22" s="107"/>
-      <c r="M22" s="107"/>
-      <c r="N22" s="161"/>
-      <c r="O22" s="162"/>
-      <c r="P22" s="82"/>
-      <c r="Q22" s="35"/>
-      <c r="R22" s="10"/>
+      <c r="F22" s="146"/>
+      <c r="G22" s="98"/>
+      <c r="H22" s="150"/>
+      <c r="I22" s="151">
+        <v>0</v>
+      </c>
+      <c r="J22" s="150"/>
+      <c r="K22" s="150"/>
+      <c r="L22" s="98"/>
+      <c r="M22" s="98"/>
+      <c r="N22" s="152"/>
+      <c r="O22" s="153"/>
+      <c r="P22" s="76"/>
+      <c r="Q22" s="33"/>
+      <c r="R22" s="1"/>
     </row>
     <row r="23" spans="1:22" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A23" s="101" t="s">
+      <c r="A23" s="92" t="s">
         <v>23</v>
       </c>
-      <c r="B23" s="99" t="s">
+      <c r="B23" s="90" t="s">
         <v>8</v>
       </c>
-      <c r="C23" s="163"/>
-      <c r="D23" s="149">
+      <c r="C23" s="154"/>
+      <c r="D23" s="140">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E23" s="150"/>
-      <c r="F23" s="204" t="s">
+      <c r="E23" s="141"/>
+      <c r="F23" s="273" t="s">
         <v>34</v>
       </c>
-      <c r="G23" s="294" t="s">
+      <c r="G23" s="190" t="s">
         <v>33</v>
       </c>
-      <c r="H23" s="295"/>
-      <c r="I23" s="77"/>
-      <c r="J23" s="78"/>
-      <c r="K23" s="280" t="s">
+      <c r="H23" s="191"/>
+      <c r="I23" s="71"/>
+      <c r="J23" s="72"/>
+      <c r="K23" s="201" t="s">
         <v>32</v>
       </c>
-      <c r="L23" s="281"/>
-      <c r="M23" s="296" t="s">
+      <c r="L23" s="202"/>
+      <c r="M23" s="192" t="s">
         <v>60</v>
       </c>
-      <c r="N23" s="161"/>
-      <c r="O23" s="293"/>
-      <c r="P23" s="292"/>
-      <c r="Q23" s="35"/>
-      <c r="R23" s="35"/>
+      <c r="N23" s="152"/>
+      <c r="O23" s="187"/>
+      <c r="P23" s="186"/>
+      <c r="Q23" s="33"/>
+      <c r="R23" s="33"/>
     </row>
     <row r="24" spans="1:22" ht="38.4" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A24" s="101" t="s">
+      <c r="A24" s="92" t="s">
         <v>24</v>
       </c>
-      <c r="B24" s="99" t="s">
+      <c r="B24" s="90" t="s">
         <v>3</v>
       </c>
-      <c r="C24" s="148"/>
-      <c r="D24" s="149">
+      <c r="C24" s="139"/>
+      <c r="D24" s="140">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E24" s="150"/>
-      <c r="F24" s="205"/>
-      <c r="G24" s="96" t="s">
+      <c r="E24" s="141"/>
+      <c r="F24" s="274"/>
+      <c r="G24" s="87" t="s">
         <v>30</v>
       </c>
-      <c r="H24" s="164">
+      <c r="H24" s="155">
         <v>1.4999999999999999E-2</v>
       </c>
-      <c r="I24" s="97"/>
-      <c r="J24" s="102"/>
-      <c r="K24" s="98" t="s">
+      <c r="I24" s="88"/>
+      <c r="J24" s="93"/>
+      <c r="K24" s="89" t="s">
         <v>31</v>
       </c>
-      <c r="L24" s="165">
+      <c r="L24" s="156">
         <v>0.01</v>
       </c>
-      <c r="M24" s="297"/>
-      <c r="N24" s="161"/>
-      <c r="O24" s="293"/>
-      <c r="P24" s="292"/>
-      <c r="Q24" s="22"/>
-      <c r="S24" s="37"/>
+      <c r="M24" s="193"/>
+      <c r="N24" s="152"/>
+      <c r="O24" s="187"/>
+      <c r="P24" s="186"/>
+      <c r="Q24" s="20"/>
+      <c r="S24" s="34"/>
       <c r="U24" s="4"/>
     </row>
     <row r="25" spans="1:22" ht="27.65" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A25" s="216" t="s">
+      <c r="A25" s="212" t="s">
         <v>71</v>
       </c>
-      <c r="B25" s="217"/>
-      <c r="C25" s="148"/>
-      <c r="D25" s="149">
+      <c r="B25" s="213"/>
+      <c r="C25" s="139"/>
+      <c r="D25" s="140">
         <f t="shared" si="5"/>
         <v>0</v>
       </c>
-      <c r="E25" s="150"/>
-      <c r="F25" s="205"/>
-      <c r="G25" s="207" t="s">
+      <c r="E25" s="141"/>
+      <c r="F25" s="274"/>
+      <c r="G25" s="276" t="s">
         <v>45</v>
       </c>
-      <c r="H25" s="220" t="s">
+      <c r="H25" s="279" t="s">
         <v>51</v>
       </c>
-      <c r="I25" s="184" t="s">
+      <c r="I25" s="291" t="s">
         <v>52</v>
       </c>
-      <c r="J25" s="185"/>
-      <c r="K25" s="192" t="s">
+      <c r="J25" s="292"/>
+      <c r="K25" s="299" t="s">
         <v>49</v>
       </c>
-      <c r="L25" s="273" t="s">
+      <c r="L25" s="252" t="s">
         <v>50</v>
       </c>
-      <c r="M25" s="244">
+      <c r="M25" s="221">
         <f>G29+L29+(L15*1%)</f>
         <v>0</v>
       </c>
-      <c r="N25" s="161"/>
-      <c r="O25" s="166"/>
-      <c r="P25" s="87"/>
+      <c r="N25" s="152"/>
+      <c r="O25" s="157"/>
+      <c r="P25" s="79"/>
       <c r="Q25" s="4"/>
-      <c r="S25" s="35"/>
+      <c r="S25" s="33"/>
     </row>
     <row r="26" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A26" s="195" t="s">
+      <c r="A26" s="302" t="s">
         <v>69</v>
       </c>
-      <c r="B26" s="196"/>
-      <c r="C26" s="181">
+      <c r="B26" s="303"/>
+      <c r="C26" s="288">
         <f>SUM(C18:C25)</f>
         <v>0</v>
       </c>
-      <c r="D26" s="251">
+      <c r="D26" s="228">
         <f>SUM(D18:D25)</f>
         <v>0</v>
       </c>
-      <c r="E26" s="150"/>
-      <c r="F26" s="205"/>
-      <c r="G26" s="208"/>
-      <c r="H26" s="221"/>
-      <c r="I26" s="186"/>
-      <c r="J26" s="187"/>
-      <c r="K26" s="193"/>
-      <c r="L26" s="274"/>
-      <c r="M26" s="245"/>
-      <c r="N26" s="161"/>
-      <c r="O26" s="167"/>
-      <c r="P26" s="88"/>
+      <c r="E26" s="141"/>
+      <c r="F26" s="274"/>
+      <c r="G26" s="277"/>
+      <c r="H26" s="280"/>
+      <c r="I26" s="293"/>
+      <c r="J26" s="294"/>
+      <c r="K26" s="300"/>
+      <c r="L26" s="253"/>
+      <c r="M26" s="222"/>
+      <c r="N26" s="152"/>
+      <c r="O26" s="158"/>
+      <c r="P26" s="80"/>
       <c r="Q26" s="4"/>
-      <c r="S26" s="35"/>
+      <c r="S26" s="33"/>
     </row>
     <row r="27" spans="1:22" ht="20.25" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A27" s="197"/>
-      <c r="B27" s="198"/>
-      <c r="C27" s="182"/>
-      <c r="D27" s="252"/>
-      <c r="E27" s="150"/>
-      <c r="F27" s="206"/>
-      <c r="G27" s="209"/>
-      <c r="H27" s="222"/>
-      <c r="I27" s="188"/>
-      <c r="J27" s="189"/>
-      <c r="K27" s="194"/>
-      <c r="L27" s="275"/>
-      <c r="M27" s="245"/>
-      <c r="N27" s="155"/>
-      <c r="O27" s="168"/>
-      <c r="P27" s="89"/>
-      <c r="Q27" s="80"/>
-      <c r="S27" s="35"/>
+      <c r="A27" s="304"/>
+      <c r="B27" s="305"/>
+      <c r="C27" s="289"/>
+      <c r="D27" s="229"/>
+      <c r="E27" s="141"/>
+      <c r="F27" s="275"/>
+      <c r="G27" s="278"/>
+      <c r="H27" s="281"/>
+      <c r="I27" s="295"/>
+      <c r="J27" s="296"/>
+      <c r="K27" s="301"/>
+      <c r="L27" s="254"/>
+      <c r="M27" s="222"/>
+      <c r="N27" s="146"/>
+      <c r="O27" s="159"/>
+      <c r="P27" s="81"/>
+      <c r="Q27" s="74"/>
+      <c r="S27" s="33"/>
     </row>
     <row r="28" spans="1:22" ht="27.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A28" s="199"/>
-      <c r="B28" s="200"/>
-      <c r="C28" s="183"/>
-      <c r="D28" s="253"/>
-      <c r="E28" s="150"/>
-      <c r="F28" s="56" t="s">
+      <c r="A28" s="306"/>
+      <c r="B28" s="307"/>
+      <c r="C28" s="290"/>
+      <c r="D28" s="230"/>
+      <c r="E28" s="141"/>
+      <c r="F28" s="52" t="s">
         <v>35</v>
       </c>
-      <c r="G28" s="169"/>
-      <c r="H28" s="170">
-        <v>0</v>
-      </c>
-      <c r="I28" s="179"/>
-      <c r="J28" s="180"/>
-      <c r="K28" s="171"/>
-      <c r="L28" s="172"/>
-      <c r="M28" s="245"/>
-      <c r="N28" s="155"/>
-      <c r="O28" s="173"/>
-      <c r="P28" s="89"/>
-      <c r="Q28" s="80"/>
-      <c r="R28" s="35"/>
+      <c r="G28" s="160"/>
+      <c r="H28" s="161">
+        <v>0</v>
+      </c>
+      <c r="I28" s="286"/>
+      <c r="J28" s="287"/>
+      <c r="K28" s="162"/>
+      <c r="L28" s="163"/>
+      <c r="M28" s="222"/>
+      <c r="N28" s="146"/>
+      <c r="O28" s="164"/>
+      <c r="P28" s="81"/>
+      <c r="Q28" s="74"/>
+      <c r="R28" s="33"/>
     </row>
     <row r="29" spans="1:22" ht="24.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.45">
-      <c r="A29" s="46"/>
-      <c r="B29" s="174"/>
-      <c r="C29" s="150"/>
-      <c r="D29" s="150"/>
-      <c r="E29" s="150"/>
-      <c r="F29" s="57" t="s">
+      <c r="A29" s="42"/>
+      <c r="B29" s="67"/>
+      <c r="C29" s="141"/>
+      <c r="D29" s="141"/>
+      <c r="E29" s="141"/>
+      <c r="F29" s="53" t="s">
         <v>36</v>
       </c>
-      <c r="G29" s="190">
+      <c r="G29" s="297">
         <f>(G28+H28)*H24</f>
         <v>0</v>
       </c>
-      <c r="H29" s="191"/>
-      <c r="I29" s="247"/>
-      <c r="J29" s="248"/>
-      <c r="K29" s="175"/>
-      <c r="L29" s="176">
+      <c r="H29" s="298"/>
+      <c r="I29" s="224"/>
+      <c r="J29" s="225"/>
+      <c r="K29" s="165"/>
+      <c r="L29" s="166">
         <f>(I28+K28+L28)*L24</f>
         <v>0</v>
       </c>
-      <c r="M29" s="246"/>
-      <c r="N29" s="155"/>
-      <c r="O29" s="91"/>
-      <c r="P29" s="91"/>
-      <c r="Q29" s="80"/>
-      <c r="R29" s="35"/>
+      <c r="M29" s="223"/>
+      <c r="N29" s="146"/>
+      <c r="O29" s="83"/>
+      <c r="P29" s="83"/>
+      <c r="Q29" s="74"/>
+      <c r="R29" s="33"/>
     </row>
     <row r="30" spans="1:22" ht="19.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.4">
-      <c r="A30" s="46"/>
-      <c r="B30" s="47"/>
-      <c r="C30" s="25"/>
-      <c r="D30" s="25"/>
-      <c r="E30" s="25"/>
-      <c r="F30" s="72"/>
-      <c r="G30" s="73"/>
-      <c r="H30" s="73"/>
-      <c r="I30" s="74"/>
-      <c r="J30" s="74"/>
-      <c r="K30" s="74"/>
-      <c r="L30" s="73"/>
-      <c r="M30" s="73"/>
-      <c r="N30" s="73"/>
-      <c r="O30" s="90"/>
-      <c r="P30" s="91"/>
-      <c r="Q30" s="81"/>
-      <c r="R30" s="35"/>
+      <c r="A30" s="42"/>
+      <c r="B30" s="43"/>
+      <c r="C30" s="23"/>
+      <c r="D30" s="23"/>
+      <c r="E30" s="23"/>
+      <c r="F30" s="67"/>
+      <c r="G30" s="68"/>
+      <c r="H30" s="68"/>
+      <c r="I30" s="69"/>
+      <c r="J30" s="69"/>
+      <c r="K30" s="69"/>
+      <c r="L30" s="68"/>
+      <c r="M30" s="68"/>
+      <c r="N30" s="68"/>
+      <c r="O30" s="82"/>
+      <c r="P30" s="83"/>
+      <c r="Q30" s="75"/>
+      <c r="R30" s="33"/>
     </row>
     <row r="31" spans="1:22" ht="34.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A31" s="46"/>
-      <c r="B31" s="178" t="s">
+      <c r="A31" s="42"/>
+      <c r="B31" s="285" t="s">
         <v>75</v>
       </c>
-      <c r="C31" s="178"/>
-      <c r="D31" s="178"/>
-      <c r="E31" s="178"/>
-      <c r="F31" s="178"/>
-      <c r="G31" s="48"/>
-      <c r="H31" s="18"/>
-      <c r="I31" s="18"/>
-      <c r="J31" s="49"/>
-      <c r="K31" s="49"/>
-      <c r="L31" s="50"/>
-      <c r="M31" s="50"/>
-      <c r="N31" s="63"/>
-      <c r="O31" s="92"/>
-      <c r="P31" s="91"/>
-      <c r="Q31" s="81"/>
-      <c r="R31" s="35"/>
+      <c r="C31" s="285"/>
+      <c r="D31" s="285"/>
+      <c r="E31" s="285"/>
+      <c r="F31" s="285"/>
+      <c r="G31" s="44"/>
+      <c r="H31" s="16"/>
+      <c r="I31" s="16"/>
+      <c r="J31" s="45"/>
+      <c r="K31" s="45"/>
+      <c r="L31" s="46"/>
+      <c r="M31" s="46"/>
+      <c r="N31" s="58"/>
+      <c r="O31" s="84"/>
+      <c r="P31" s="83"/>
+      <c r="Q31" s="75"/>
+      <c r="R31" s="33"/>
     </row>
-    <row r="32" spans="1:22" s="40" customFormat="1" ht="160.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A32" s="66" t="s">
+    <row r="32" spans="1:22" s="24" customFormat="1" ht="160.5" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A32" s="61" t="s">
         <v>39</v>
       </c>
-      <c r="B32" s="178"/>
-      <c r="C32" s="178"/>
-      <c r="D32" s="178"/>
-      <c r="E32" s="178"/>
-      <c r="F32" s="178"/>
-      <c r="G32" s="67" t="s">
+      <c r="B32" s="285"/>
+      <c r="C32" s="285"/>
+      <c r="D32" s="285"/>
+      <c r="E32" s="285"/>
+      <c r="F32" s="285"/>
+      <c r="G32" s="62" t="s">
         <v>76</v>
       </c>
-      <c r="H32" s="64" t="s">
+      <c r="H32" s="59" t="s">
         <v>77</v>
       </c>
-      <c r="I32" s="79"/>
-      <c r="K32" s="177" t="s">
+      <c r="I32" s="73"/>
+      <c r="K32" s="284" t="s">
         <v>40</v>
       </c>
-      <c r="L32" s="177"/>
-      <c r="M32" s="65"/>
-      <c r="N32" s="62"/>
-      <c r="O32" s="93"/>
-      <c r="P32" s="94"/>
-      <c r="Q32" s="45"/>
-      <c r="R32" s="45"/>
+      <c r="L32" s="284"/>
+      <c r="M32" s="60"/>
+      <c r="N32" s="57"/>
+      <c r="O32" s="85"/>
+      <c r="Q32" s="41"/>
+      <c r="R32" s="41"/>
     </row>
     <row r="33" spans="1:14" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
@@ -5786,7 +5726,7 @@
       <c r="K33" s="3"/>
       <c r="L33" s="3"/>
       <c r="M33" s="3"/>
-      <c r="N33" s="21"/>
+      <c r="N33" s="19"/>
     </row>
     <row r="34" spans="1:14" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A34" s="8" t="s">
@@ -5805,42 +5745,42 @@
       <c r="F34" s="8" t="s">
         <v>16</v>
       </c>
-      <c r="G34" s="39" t="s">
+      <c r="G34" s="36" t="s">
         <v>9</v>
       </c>
-      <c r="H34" s="40"/>
-      <c r="I34" s="41"/>
-      <c r="J34" s="40"/>
-      <c r="K34" s="42" t="s">
+      <c r="H34" s="24"/>
+      <c r="I34" s="37"/>
+      <c r="J34" s="24"/>
+      <c r="K34" s="38" t="s">
         <v>13</v>
       </c>
-      <c r="L34" s="43"/>
-      <c r="M34" s="44"/>
+      <c r="L34" s="39"/>
+      <c r="M34" s="40"/>
       <c r="N34" s="4"/>
     </row>
     <row r="35" spans="1:14" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A35" s="14" t="e">
+      <c r="A35" s="12" t="e">
         <v>#REF!</v>
       </c>
-      <c r="B35" s="14" t="e">
+      <c r="B35" s="12" t="e">
         <v>#REF!</v>
       </c>
-      <c r="C35" s="15" t="e">
+      <c r="C35" s="13" t="e">
         <v>#REF!</v>
       </c>
-      <c r="D35" s="15">
+      <c r="D35" s="13">
         <v>53854214514</v>
       </c>
-      <c r="E35" s="15"/>
-      <c r="F35" s="16" t="e">
+      <c r="E35" s="13"/>
+      <c r="F35" s="14" t="e">
         <v>#REF!</v>
       </c>
-      <c r="G35" s="28" t="s">
+      <c r="G35" s="26" t="s">
         <v>9</v>
       </c>
-      <c r="H35" s="21"/>
+      <c r="H35" s="19"/>
       <c r="I35" s="4"/>
-      <c r="K35" s="29" t="s">
+      <c r="K35" s="27" t="s">
         <v>13</v>
       </c>
       <c r="L35" s="1"/>
@@ -5854,44 +5794,44 @@
       <c r="B36" s="5" t="e">
         <v>#REF!</v>
       </c>
-      <c r="C36" s="11" t="e">
+      <c r="C36" s="5" t="e">
         <v>#REF!</v>
       </c>
-      <c r="D36" s="11">
-        <v>0</v>
-      </c>
-      <c r="E36" s="11"/>
-      <c r="F36" s="11" t="e">
+      <c r="D36" s="5">
+        <v>0</v>
+      </c>
+      <c r="E36" s="5"/>
+      <c r="F36" s="5" t="e">
         <v>#REF!</v>
       </c>
-      <c r="G36" s="24"/>
+      <c r="G36" s="22"/>
       <c r="H36" s="1"/>
       <c r="I36" s="7"/>
       <c r="J36" s="1"/>
       <c r="K36" s="1"/>
     </row>
     <row r="37" spans="1:14" ht="31.5" hidden="1" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C37" s="13" t="e">
+      <c r="C37" s="11" t="e">
         <v>#REF!</v>
       </c>
-      <c r="F37" s="10" t="s">
+      <c r="F37" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G37" s="23"/>
-      <c r="H37" s="24"/>
+      <c r="G37" s="21"/>
+      <c r="H37" s="22"/>
     </row>
     <row r="38" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="B38" s="10" t="s">
+      <c r="B38" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="G38" s="11"/>
-      <c r="H38" s="10"/>
+      <c r="G38" s="5"/>
+      <c r="H38" s="1"/>
     </row>
     <row r="39" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="C39" s="34"/>
+      <c r="C39" s="32"/>
     </row>
     <row r="40" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A40" s="34"/>
+      <c r="A40" s="32"/>
     </row>
     <row r="41" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A41"/>
@@ -5902,13 +5842,13 @@
       <c r="B42"/>
     </row>
     <row r="43" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A43" s="95"/>
+      <c r="A43" s="86"/>
       <c r="B43"/>
     </row>
     <row r="44" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A44" s="95"/>
+      <c r="A44" s="86"/>
       <c r="B44"/>
-      <c r="C44" s="34"/>
+      <c r="C44" s="32"/>
     </row>
     <row r="45" spans="1:14" ht="31.5" customHeight="1" x14ac:dyDescent="0.4">
       <c r="A45"/>
@@ -5918,12 +5858,62 @@
     </row>
   </sheetData>
   <mergeCells count="78">
-    <mergeCell ref="P23:P24"/>
-    <mergeCell ref="O23:O24"/>
-    <mergeCell ref="K19:L19"/>
-    <mergeCell ref="G23:H23"/>
-    <mergeCell ref="M23:M24"/>
-    <mergeCell ref="G21:I21"/>
+    <mergeCell ref="K32:L32"/>
+    <mergeCell ref="B31:F32"/>
+    <mergeCell ref="I28:J28"/>
+    <mergeCell ref="C26:C28"/>
+    <mergeCell ref="I25:J27"/>
+    <mergeCell ref="G29:H29"/>
+    <mergeCell ref="K25:K27"/>
+    <mergeCell ref="A26:B28"/>
+    <mergeCell ref="J11:K11"/>
+    <mergeCell ref="J12:K12"/>
+    <mergeCell ref="B6:B8"/>
+    <mergeCell ref="F23:F27"/>
+    <mergeCell ref="G25:G27"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="J8:K8"/>
+    <mergeCell ref="A25:B25"/>
+    <mergeCell ref="G11:H11"/>
+    <mergeCell ref="G10:H10"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="J6:K6"/>
+    <mergeCell ref="H25:H27"/>
+    <mergeCell ref="G14:H14"/>
+    <mergeCell ref="A2:B3"/>
+    <mergeCell ref="J7:K7"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="J9:K9"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="C2:C3"/>
+    <mergeCell ref="D2:E3"/>
+    <mergeCell ref="G4:H4"/>
+    <mergeCell ref="A6:A8"/>
+    <mergeCell ref="G6:H6"/>
+    <mergeCell ref="D5:E5"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="A4:A5"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="M25:M29"/>
+    <mergeCell ref="I29:J29"/>
+    <mergeCell ref="K17:L17"/>
+    <mergeCell ref="D26:D28"/>
+    <mergeCell ref="F2:F3"/>
+    <mergeCell ref="G2:H3"/>
+    <mergeCell ref="D14:E14"/>
+    <mergeCell ref="J3:K3"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="J14:K14"/>
+    <mergeCell ref="I2:M2"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="D8:E8"/>
+    <mergeCell ref="J10:K10"/>
+    <mergeCell ref="D11:E11"/>
+    <mergeCell ref="L25:L27"/>
     <mergeCell ref="D12:E12"/>
     <mergeCell ref="G12:H12"/>
     <mergeCell ref="K23:L23"/>
@@ -5940,62 +5930,12 @@
     <mergeCell ref="D13:E13"/>
     <mergeCell ref="G13:H13"/>
     <mergeCell ref="J13:K13"/>
-    <mergeCell ref="M25:M29"/>
-    <mergeCell ref="I29:J29"/>
-    <mergeCell ref="K17:L17"/>
-    <mergeCell ref="D26:D28"/>
-    <mergeCell ref="F2:F3"/>
-    <mergeCell ref="G2:H3"/>
-    <mergeCell ref="D14:E14"/>
-    <mergeCell ref="J3:K3"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="J14:K14"/>
-    <mergeCell ref="I2:M2"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="D8:E8"/>
-    <mergeCell ref="J10:K10"/>
-    <mergeCell ref="D11:E11"/>
-    <mergeCell ref="L25:L27"/>
-    <mergeCell ref="A2:B3"/>
-    <mergeCell ref="J7:K7"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="J9:K9"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="C2:C3"/>
-    <mergeCell ref="D2:E3"/>
-    <mergeCell ref="G4:H4"/>
-    <mergeCell ref="A6:A8"/>
-    <mergeCell ref="G6:H6"/>
-    <mergeCell ref="D5:E5"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="A4:A5"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="J11:K11"/>
-    <mergeCell ref="J12:K12"/>
-    <mergeCell ref="B6:B8"/>
-    <mergeCell ref="F23:F27"/>
-    <mergeCell ref="G25:G27"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="J8:K8"/>
-    <mergeCell ref="A25:B25"/>
-    <mergeCell ref="G11:H11"/>
-    <mergeCell ref="G10:H10"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="J6:K6"/>
-    <mergeCell ref="H25:H27"/>
-    <mergeCell ref="G14:H14"/>
-    <mergeCell ref="K32:L32"/>
-    <mergeCell ref="B31:F32"/>
-    <mergeCell ref="I28:J28"/>
-    <mergeCell ref="C26:C28"/>
-    <mergeCell ref="I25:J27"/>
-    <mergeCell ref="G29:H29"/>
-    <mergeCell ref="K25:K27"/>
-    <mergeCell ref="A26:B28"/>
+    <mergeCell ref="P23:P24"/>
+    <mergeCell ref="O23:O24"/>
+    <mergeCell ref="K19:L19"/>
+    <mergeCell ref="G23:H23"/>
+    <mergeCell ref="M23:M24"/>
+    <mergeCell ref="G21:I21"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
@@ -6011,14 +5951,14 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor indexed="52"/>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
   <dimension ref="A1:CR231"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+    <sheetView zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
       <pane xSplit="10" ySplit="2" topLeftCell="K3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="K1" sqref="K1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
@@ -6027,556 +5967,554 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="17" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="12.1796875" style="301" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16" style="310" customWidth="1"/>
-    <col min="3" max="4" width="8.1796875" style="308" customWidth="1"/>
-    <col min="5" max="5" width="19.6328125" style="306" customWidth="1"/>
-    <col min="6" max="6" width="17.6328125" style="307" customWidth="1"/>
-    <col min="7" max="7" width="9" style="308" customWidth="1"/>
-    <col min="8" max="8" width="13.7265625" style="309" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="9" style="308" customWidth="1"/>
-    <col min="10" max="11" width="13.08984375" style="308" customWidth="1"/>
-    <col min="12" max="12" width="15.6328125" style="307" customWidth="1"/>
-    <col min="13" max="13" width="18.36328125" style="307" customWidth="1"/>
-    <col min="14" max="14" width="16.90625" style="307" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="17" style="307" customWidth="1"/>
-    <col min="16" max="16" width="14.1796875" style="307" customWidth="1"/>
-    <col min="17" max="17" width="16.36328125" style="307" customWidth="1"/>
-    <col min="18" max="18" width="52.36328125" style="306" customWidth="1"/>
-    <col min="19" max="19" width="21.81640625" style="305" customWidth="1"/>
-    <col min="20" max="20" width="42.1796875" style="304" customWidth="1"/>
-    <col min="21" max="21" width="17" style="303" customWidth="1"/>
-    <col min="22" max="22" width="17" style="302" customWidth="1"/>
-    <col min="23" max="23" width="12.1796875" style="302" bestFit="1" customWidth="1"/>
-    <col min="24" max="96" width="9" style="302"/>
-    <col min="97" max="16384" width="9" style="301"/>
+    <col min="1" max="1" width="12.1796875" style="167" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16" style="167" customWidth="1"/>
+    <col min="3" max="4" width="8.1796875" style="168" customWidth="1"/>
+    <col min="5" max="5" width="19.6328125" style="171" customWidth="1"/>
+    <col min="6" max="6" width="17.6328125" style="172" customWidth="1"/>
+    <col min="7" max="7" width="9" style="168" customWidth="1"/>
+    <col min="8" max="8" width="13.7265625" style="173" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9" style="168" customWidth="1"/>
+    <col min="10" max="11" width="13.08984375" style="168" customWidth="1"/>
+    <col min="12" max="12" width="15.6328125" style="172" customWidth="1"/>
+    <col min="13" max="13" width="18.36328125" style="172" customWidth="1"/>
+    <col min="14" max="14" width="16.90625" style="172" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="17" style="172" customWidth="1"/>
+    <col min="16" max="16" width="14.1796875" style="172" customWidth="1"/>
+    <col min="17" max="17" width="16.36328125" style="172" customWidth="1"/>
+    <col min="18" max="18" width="52.36328125" style="171" customWidth="1"/>
+    <col min="19" max="19" width="21.81640625" style="170" customWidth="1"/>
+    <col min="20" max="20" width="42.1796875" style="169" customWidth="1"/>
+    <col min="21" max="21" width="17" style="168" customWidth="1"/>
+    <col min="22" max="22" width="17" style="167" customWidth="1"/>
+    <col min="23" max="23" width="12.1796875" style="167" bestFit="1" customWidth="1"/>
+    <col min="24" max="16384" width="9" style="167"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:96" ht="19.5" x14ac:dyDescent="0.45">
-      <c r="B1" s="322" t="s">
+      <c r="B1" s="185" t="s">
         <v>100</v>
       </c>
-      <c r="T1" s="321" t="s">
+      <c r="T1" s="184" t="s">
         <v>99</v>
       </c>
-      <c r="CR1" s="301"/>
     </row>
-    <row r="2" spans="1:96" s="312" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
-      <c r="A2" s="312" t="s">
+    <row r="2" spans="1:96" s="175" customFormat="1" ht="18" customHeight="1" x14ac:dyDescent="0.4">
+      <c r="A2" s="175" t="s">
         <v>98</v>
       </c>
-      <c r="B2" s="317" t="s">
+      <c r="B2" s="180" t="s">
         <v>97</v>
       </c>
-      <c r="C2" s="317" t="s">
+      <c r="C2" s="180" t="s">
         <v>96</v>
       </c>
-      <c r="D2" s="317" t="s">
+      <c r="D2" s="180" t="s">
         <v>95</v>
       </c>
-      <c r="E2" s="317" t="s">
+      <c r="E2" s="180" t="s">
         <v>94</v>
       </c>
-      <c r="F2" s="316" t="s">
+      <c r="F2" s="179" t="s">
         <v>93</v>
       </c>
-      <c r="G2" s="320" t="s">
+      <c r="G2" s="183" t="s">
         <v>92</v>
       </c>
-      <c r="H2" s="317" t="s">
+      <c r="H2" s="180" t="s">
         <v>91</v>
       </c>
-      <c r="I2" s="317" t="s">
+      <c r="I2" s="180" t="s">
         <v>90</v>
       </c>
-      <c r="J2" s="317" t="s">
+      <c r="J2" s="180" t="s">
         <v>89</v>
       </c>
-      <c r="K2" s="319" t="s">
+      <c r="K2" s="182" t="s">
         <v>88</v>
       </c>
-      <c r="L2" s="318" t="s">
+      <c r="L2" s="181" t="s">
         <v>87</v>
       </c>
-      <c r="M2" s="318" t="s">
+      <c r="M2" s="181" t="s">
         <v>86</v>
       </c>
-      <c r="N2" s="318" t="s">
+      <c r="N2" s="181" t="s">
         <v>85</v>
       </c>
-      <c r="O2" s="318" t="s">
+      <c r="O2" s="181" t="s">
         <v>84</v>
       </c>
-      <c r="P2" s="318" t="s">
+      <c r="P2" s="181" t="s">
         <v>83</v>
       </c>
-      <c r="Q2" s="318" t="s">
+      <c r="Q2" s="181" t="s">
         <v>82</v>
       </c>
-      <c r="R2" s="317" t="s">
+      <c r="R2" s="180" t="s">
         <v>81</v>
       </c>
-      <c r="S2" s="316" t="s">
+      <c r="S2" s="179" t="s">
         <v>80</v>
       </c>
-      <c r="T2" s="315" t="s">
+      <c r="T2" s="178" t="s">
         <v>79</v>
       </c>
-      <c r="U2" s="314" t="s">
+      <c r="U2" s="177" t="s">
         <v>78</v>
       </c>
-      <c r="V2" s="313"/>
-      <c r="W2" s="313"/>
-      <c r="X2" s="313"/>
-      <c r="Y2" s="313"/>
-      <c r="Z2" s="313"/>
-      <c r="AA2" s="313"/>
-      <c r="AB2" s="313"/>
-      <c r="AC2" s="313"/>
-      <c r="AD2" s="313"/>
-      <c r="AE2" s="313"/>
-      <c r="AF2" s="313"/>
-      <c r="AG2" s="313"/>
-      <c r="AH2" s="313"/>
-      <c r="AI2" s="313"/>
-      <c r="AJ2" s="313"/>
-      <c r="AK2" s="313"/>
-      <c r="AL2" s="313"/>
-      <c r="AM2" s="313"/>
-      <c r="AN2" s="313"/>
-      <c r="AO2" s="313"/>
-      <c r="AP2" s="313"/>
-      <c r="AQ2" s="313"/>
-      <c r="AR2" s="313"/>
-      <c r="AS2" s="313"/>
-      <c r="AT2" s="313"/>
-      <c r="AU2" s="313"/>
-      <c r="AV2" s="313"/>
-      <c r="AW2" s="313"/>
-      <c r="AX2" s="313"/>
-      <c r="AY2" s="313"/>
-      <c r="AZ2" s="313"/>
-      <c r="BA2" s="313"/>
-      <c r="BB2" s="313"/>
-      <c r="BC2" s="313"/>
-      <c r="BD2" s="313"/>
-      <c r="BE2" s="313"/>
-      <c r="BF2" s="313"/>
-      <c r="BG2" s="313"/>
-      <c r="BH2" s="313"/>
-      <c r="BI2" s="313"/>
-      <c r="BJ2" s="313"/>
-      <c r="BK2" s="313"/>
-      <c r="BL2" s="313"/>
-      <c r="BM2" s="313"/>
-      <c r="BN2" s="313"/>
-      <c r="BO2" s="313"/>
-      <c r="BP2" s="313"/>
-      <c r="BQ2" s="313"/>
-      <c r="BR2" s="313"/>
-      <c r="BS2" s="313"/>
-      <c r="BT2" s="313"/>
-      <c r="BU2" s="313"/>
-      <c r="BV2" s="313"/>
-      <c r="BW2" s="313"/>
-      <c r="BX2" s="313"/>
-      <c r="BY2" s="313"/>
-      <c r="BZ2" s="313"/>
-      <c r="CA2" s="313"/>
-      <c r="CB2" s="313"/>
-      <c r="CC2" s="313"/>
-      <c r="CD2" s="313"/>
-      <c r="CE2" s="313"/>
-      <c r="CF2" s="313"/>
-      <c r="CG2" s="313"/>
-      <c r="CH2" s="313"/>
-      <c r="CI2" s="313"/>
-      <c r="CJ2" s="313"/>
-      <c r="CK2" s="313"/>
-      <c r="CL2" s="313"/>
-      <c r="CM2" s="313"/>
-      <c r="CN2" s="313"/>
-      <c r="CO2" s="313"/>
-      <c r="CP2" s="313"/>
-      <c r="CQ2" s="313"/>
-      <c r="CR2" s="313"/>
+      <c r="V2" s="176"/>
+      <c r="W2" s="176"/>
+      <c r="X2" s="176"/>
+      <c r="Y2" s="176"/>
+      <c r="Z2" s="176"/>
+      <c r="AA2" s="176"/>
+      <c r="AB2" s="176"/>
+      <c r="AC2" s="176"/>
+      <c r="AD2" s="176"/>
+      <c r="AE2" s="176"/>
+      <c r="AF2" s="176"/>
+      <c r="AG2" s="176"/>
+      <c r="AH2" s="176"/>
+      <c r="AI2" s="176"/>
+      <c r="AJ2" s="176"/>
+      <c r="AK2" s="176"/>
+      <c r="AL2" s="176"/>
+      <c r="AM2" s="176"/>
+      <c r="AN2" s="176"/>
+      <c r="AO2" s="176"/>
+      <c r="AP2" s="176"/>
+      <c r="AQ2" s="176"/>
+      <c r="AR2" s="176"/>
+      <c r="AS2" s="176"/>
+      <c r="AT2" s="176"/>
+      <c r="AU2" s="176"/>
+      <c r="AV2" s="176"/>
+      <c r="AW2" s="176"/>
+      <c r="AX2" s="176"/>
+      <c r="AY2" s="176"/>
+      <c r="AZ2" s="176"/>
+      <c r="BA2" s="176"/>
+      <c r="BB2" s="176"/>
+      <c r="BC2" s="176"/>
+      <c r="BD2" s="176"/>
+      <c r="BE2" s="176"/>
+      <c r="BF2" s="176"/>
+      <c r="BG2" s="176"/>
+      <c r="BH2" s="176"/>
+      <c r="BI2" s="176"/>
+      <c r="BJ2" s="176"/>
+      <c r="BK2" s="176"/>
+      <c r="BL2" s="176"/>
+      <c r="BM2" s="176"/>
+      <c r="BN2" s="176"/>
+      <c r="BO2" s="176"/>
+      <c r="BP2" s="176"/>
+      <c r="BQ2" s="176"/>
+      <c r="BR2" s="176"/>
+      <c r="BS2" s="176"/>
+      <c r="BT2" s="176"/>
+      <c r="BU2" s="176"/>
+      <c r="BV2" s="176"/>
+      <c r="BW2" s="176"/>
+      <c r="BX2" s="176"/>
+      <c r="BY2" s="176"/>
+      <c r="BZ2" s="176"/>
+      <c r="CA2" s="176"/>
+      <c r="CB2" s="176"/>
+      <c r="CC2" s="176"/>
+      <c r="CD2" s="176"/>
+      <c r="CE2" s="176"/>
+      <c r="CF2" s="176"/>
+      <c r="CG2" s="176"/>
+      <c r="CH2" s="176"/>
+      <c r="CI2" s="176"/>
+      <c r="CJ2" s="176"/>
+      <c r="CK2" s="176"/>
+      <c r="CL2" s="176"/>
+      <c r="CM2" s="176"/>
+      <c r="CN2" s="176"/>
+      <c r="CO2" s="176"/>
+      <c r="CP2" s="176"/>
+      <c r="CQ2" s="176"/>
+      <c r="CR2" s="176"/>
     </row>
-    <row r="81" spans="2:96" s="311" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B81" s="310"/>
-      <c r="C81" s="308"/>
-      <c r="D81" s="308"/>
-      <c r="E81" s="306"/>
-      <c r="F81" s="307"/>
-      <c r="G81" s="308"/>
-      <c r="H81" s="309"/>
-      <c r="I81" s="308"/>
-      <c r="J81" s="308"/>
-      <c r="K81" s="308"/>
-      <c r="L81" s="307"/>
-      <c r="M81" s="307"/>
-      <c r="N81" s="307"/>
-      <c r="O81" s="307"/>
-      <c r="P81" s="307"/>
-      <c r="Q81" s="307"/>
-      <c r="R81" s="306"/>
-      <c r="S81" s="305"/>
-      <c r="T81" s="304"/>
-      <c r="U81" s="303"/>
-      <c r="V81" s="302"/>
-      <c r="W81" s="302"/>
-      <c r="X81" s="302"/>
-      <c r="Y81" s="302"/>
-      <c r="Z81" s="302"/>
-      <c r="AA81" s="302"/>
-      <c r="AB81" s="302"/>
-      <c r="AC81" s="302"/>
-      <c r="AD81" s="302"/>
-      <c r="AE81" s="302"/>
-      <c r="AF81" s="302"/>
-      <c r="AG81" s="302"/>
-      <c r="AH81" s="302"/>
-      <c r="AI81" s="302"/>
-      <c r="AJ81" s="302"/>
-      <c r="AK81" s="302"/>
-      <c r="AL81" s="302"/>
-      <c r="AM81" s="302"/>
-      <c r="AN81" s="302"/>
-      <c r="AO81" s="302"/>
-      <c r="AP81" s="302"/>
-      <c r="AQ81" s="302"/>
-      <c r="AR81" s="302"/>
-      <c r="AS81" s="302"/>
-      <c r="AT81" s="302"/>
-      <c r="AU81" s="302"/>
-      <c r="AV81" s="302"/>
-      <c r="AW81" s="302"/>
-      <c r="AX81" s="302"/>
-      <c r="AY81" s="302"/>
-      <c r="AZ81" s="302"/>
-      <c r="BA81" s="302"/>
-      <c r="BB81" s="302"/>
-      <c r="BC81" s="302"/>
-      <c r="BD81" s="302"/>
-      <c r="BE81" s="302"/>
-      <c r="BF81" s="302"/>
-      <c r="BG81" s="302"/>
-      <c r="BH81" s="302"/>
-      <c r="BI81" s="302"/>
-      <c r="BJ81" s="302"/>
-      <c r="BK81" s="302"/>
-      <c r="BL81" s="302"/>
-      <c r="BM81" s="302"/>
-      <c r="BN81" s="302"/>
-      <c r="BO81" s="302"/>
-      <c r="BP81" s="302"/>
-      <c r="BQ81" s="302"/>
-      <c r="BR81" s="302"/>
-      <c r="BS81" s="302"/>
-      <c r="BT81" s="302"/>
-      <c r="BU81" s="302"/>
-      <c r="BV81" s="302"/>
-      <c r="BW81" s="302"/>
-      <c r="BX81" s="302"/>
-      <c r="BY81" s="302"/>
-      <c r="BZ81" s="302"/>
-      <c r="CA81" s="302"/>
-      <c r="CB81" s="302"/>
-      <c r="CC81" s="302"/>
-      <c r="CD81" s="302"/>
-      <c r="CE81" s="302"/>
-      <c r="CF81" s="302"/>
-      <c r="CG81" s="302"/>
-      <c r="CH81" s="302"/>
-      <c r="CI81" s="302"/>
-      <c r="CJ81" s="302"/>
-      <c r="CK81" s="302"/>
-      <c r="CL81" s="302"/>
-      <c r="CM81" s="302"/>
-      <c r="CN81" s="302"/>
-      <c r="CO81" s="302"/>
-      <c r="CP81" s="302"/>
-      <c r="CQ81" s="302"/>
-      <c r="CR81" s="302"/>
+    <row r="81" spans="2:96" s="174" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B81" s="167"/>
+      <c r="C81" s="168"/>
+      <c r="D81" s="168"/>
+      <c r="E81" s="171"/>
+      <c r="F81" s="172"/>
+      <c r="G81" s="168"/>
+      <c r="H81" s="173"/>
+      <c r="I81" s="168"/>
+      <c r="J81" s="168"/>
+      <c r="K81" s="168"/>
+      <c r="L81" s="172"/>
+      <c r="M81" s="172"/>
+      <c r="N81" s="172"/>
+      <c r="O81" s="172"/>
+      <c r="P81" s="172"/>
+      <c r="Q81" s="172"/>
+      <c r="R81" s="171"/>
+      <c r="S81" s="170"/>
+      <c r="T81" s="169"/>
+      <c r="U81" s="168"/>
+      <c r="V81" s="167"/>
+      <c r="W81" s="167"/>
+      <c r="X81" s="167"/>
+      <c r="Y81" s="167"/>
+      <c r="Z81" s="167"/>
+      <c r="AA81" s="167"/>
+      <c r="AB81" s="167"/>
+      <c r="AC81" s="167"/>
+      <c r="AD81" s="167"/>
+      <c r="AE81" s="167"/>
+      <c r="AF81" s="167"/>
+      <c r="AG81" s="167"/>
+      <c r="AH81" s="167"/>
+      <c r="AI81" s="167"/>
+      <c r="AJ81" s="167"/>
+      <c r="AK81" s="167"/>
+      <c r="AL81" s="167"/>
+      <c r="AM81" s="167"/>
+      <c r="AN81" s="167"/>
+      <c r="AO81" s="167"/>
+      <c r="AP81" s="167"/>
+      <c r="AQ81" s="167"/>
+      <c r="AR81" s="167"/>
+      <c r="AS81" s="167"/>
+      <c r="AT81" s="167"/>
+      <c r="AU81" s="167"/>
+      <c r="AV81" s="167"/>
+      <c r="AW81" s="167"/>
+      <c r="AX81" s="167"/>
+      <c r="AY81" s="167"/>
+      <c r="AZ81" s="167"/>
+      <c r="BA81" s="167"/>
+      <c r="BB81" s="167"/>
+      <c r="BC81" s="167"/>
+      <c r="BD81" s="167"/>
+      <c r="BE81" s="167"/>
+      <c r="BF81" s="167"/>
+      <c r="BG81" s="167"/>
+      <c r="BH81" s="167"/>
+      <c r="BI81" s="167"/>
+      <c r="BJ81" s="167"/>
+      <c r="BK81" s="167"/>
+      <c r="BL81" s="167"/>
+      <c r="BM81" s="167"/>
+      <c r="BN81" s="167"/>
+      <c r="BO81" s="167"/>
+      <c r="BP81" s="167"/>
+      <c r="BQ81" s="167"/>
+      <c r="BR81" s="167"/>
+      <c r="BS81" s="167"/>
+      <c r="BT81" s="167"/>
+      <c r="BU81" s="167"/>
+      <c r="BV81" s="167"/>
+      <c r="BW81" s="167"/>
+      <c r="BX81" s="167"/>
+      <c r="BY81" s="167"/>
+      <c r="BZ81" s="167"/>
+      <c r="CA81" s="167"/>
+      <c r="CB81" s="167"/>
+      <c r="CC81" s="167"/>
+      <c r="CD81" s="167"/>
+      <c r="CE81" s="167"/>
+      <c r="CF81" s="167"/>
+      <c r="CG81" s="167"/>
+      <c r="CH81" s="167"/>
+      <c r="CI81" s="167"/>
+      <c r="CJ81" s="167"/>
+      <c r="CK81" s="167"/>
+      <c r="CL81" s="167"/>
+      <c r="CM81" s="167"/>
+      <c r="CN81" s="167"/>
+      <c r="CO81" s="167"/>
+      <c r="CP81" s="167"/>
+      <c r="CQ81" s="167"/>
+      <c r="CR81" s="167"/>
     </row>
-    <row r="83" spans="2:96" s="311" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B83" s="310"/>
-      <c r="C83" s="308"/>
-      <c r="D83" s="308"/>
-      <c r="E83" s="306"/>
-      <c r="F83" s="307"/>
-      <c r="G83" s="308"/>
-      <c r="H83" s="309"/>
-      <c r="I83" s="308"/>
-      <c r="J83" s="308"/>
-      <c r="K83" s="308"/>
-      <c r="L83" s="307"/>
-      <c r="M83" s="307"/>
-      <c r="N83" s="307"/>
-      <c r="O83" s="307"/>
-      <c r="P83" s="307"/>
-      <c r="Q83" s="307"/>
-      <c r="R83" s="306"/>
-      <c r="S83" s="305"/>
-      <c r="T83" s="304"/>
-      <c r="U83" s="303"/>
-      <c r="V83" s="302"/>
-      <c r="W83" s="302"/>
-      <c r="X83" s="302"/>
-      <c r="Y83" s="302"/>
-      <c r="Z83" s="302"/>
-      <c r="AA83" s="302"/>
-      <c r="AB83" s="302"/>
-      <c r="AC83" s="302"/>
-      <c r="AD83" s="302"/>
-      <c r="AE83" s="302"/>
-      <c r="AF83" s="302"/>
-      <c r="AG83" s="302"/>
-      <c r="AH83" s="302"/>
-      <c r="AI83" s="302"/>
-      <c r="AJ83" s="302"/>
-      <c r="AK83" s="302"/>
-      <c r="AL83" s="302"/>
-      <c r="AM83" s="302"/>
-      <c r="AN83" s="302"/>
-      <c r="AO83" s="302"/>
-      <c r="AP83" s="302"/>
-      <c r="AQ83" s="302"/>
-      <c r="AR83" s="302"/>
-      <c r="AS83" s="302"/>
-      <c r="AT83" s="302"/>
-      <c r="AU83" s="302"/>
-      <c r="AV83" s="302"/>
-      <c r="AW83" s="302"/>
-      <c r="AX83" s="302"/>
-      <c r="AY83" s="302"/>
-      <c r="AZ83" s="302"/>
-      <c r="BA83" s="302"/>
-      <c r="BB83" s="302"/>
-      <c r="BC83" s="302"/>
-      <c r="BD83" s="302"/>
-      <c r="BE83" s="302"/>
-      <c r="BF83" s="302"/>
-      <c r="BG83" s="302"/>
-      <c r="BH83" s="302"/>
-      <c r="BI83" s="302"/>
-      <c r="BJ83" s="302"/>
-      <c r="BK83" s="302"/>
-      <c r="BL83" s="302"/>
-      <c r="BM83" s="302"/>
-      <c r="BN83" s="302"/>
-      <c r="BO83" s="302"/>
-      <c r="BP83" s="302"/>
-      <c r="BQ83" s="302"/>
-      <c r="BR83" s="302"/>
-      <c r="BS83" s="302"/>
-      <c r="BT83" s="302"/>
-      <c r="BU83" s="302"/>
-      <c r="BV83" s="302"/>
-      <c r="BW83" s="302"/>
-      <c r="BX83" s="302"/>
-      <c r="BY83" s="302"/>
-      <c r="BZ83" s="302"/>
-      <c r="CA83" s="302"/>
-      <c r="CB83" s="302"/>
-      <c r="CC83" s="302"/>
-      <c r="CD83" s="302"/>
-      <c r="CE83" s="302"/>
-      <c r="CF83" s="302"/>
-      <c r="CG83" s="302"/>
-      <c r="CH83" s="302"/>
-      <c r="CI83" s="302"/>
-      <c r="CJ83" s="302"/>
-      <c r="CK83" s="302"/>
-      <c r="CL83" s="302"/>
-      <c r="CM83" s="302"/>
-      <c r="CN83" s="302"/>
-      <c r="CO83" s="302"/>
-      <c r="CP83" s="302"/>
-      <c r="CQ83" s="302"/>
-      <c r="CR83" s="302"/>
+    <row r="83" spans="2:96" s="174" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B83" s="167"/>
+      <c r="C83" s="168"/>
+      <c r="D83" s="168"/>
+      <c r="E83" s="171"/>
+      <c r="F83" s="172"/>
+      <c r="G83" s="168"/>
+      <c r="H83" s="173"/>
+      <c r="I83" s="168"/>
+      <c r="J83" s="168"/>
+      <c r="K83" s="168"/>
+      <c r="L83" s="172"/>
+      <c r="M83" s="172"/>
+      <c r="N83" s="172"/>
+      <c r="O83" s="172"/>
+      <c r="P83" s="172"/>
+      <c r="Q83" s="172"/>
+      <c r="R83" s="171"/>
+      <c r="S83" s="170"/>
+      <c r="T83" s="169"/>
+      <c r="U83" s="168"/>
+      <c r="V83" s="167"/>
+      <c r="W83" s="167"/>
+      <c r="X83" s="167"/>
+      <c r="Y83" s="167"/>
+      <c r="Z83" s="167"/>
+      <c r="AA83" s="167"/>
+      <c r="AB83" s="167"/>
+      <c r="AC83" s="167"/>
+      <c r="AD83" s="167"/>
+      <c r="AE83" s="167"/>
+      <c r="AF83" s="167"/>
+      <c r="AG83" s="167"/>
+      <c r="AH83" s="167"/>
+      <c r="AI83" s="167"/>
+      <c r="AJ83" s="167"/>
+      <c r="AK83" s="167"/>
+      <c r="AL83" s="167"/>
+      <c r="AM83" s="167"/>
+      <c r="AN83" s="167"/>
+      <c r="AO83" s="167"/>
+      <c r="AP83" s="167"/>
+      <c r="AQ83" s="167"/>
+      <c r="AR83" s="167"/>
+      <c r="AS83" s="167"/>
+      <c r="AT83" s="167"/>
+      <c r="AU83" s="167"/>
+      <c r="AV83" s="167"/>
+      <c r="AW83" s="167"/>
+      <c r="AX83" s="167"/>
+      <c r="AY83" s="167"/>
+      <c r="AZ83" s="167"/>
+      <c r="BA83" s="167"/>
+      <c r="BB83" s="167"/>
+      <c r="BC83" s="167"/>
+      <c r="BD83" s="167"/>
+      <c r="BE83" s="167"/>
+      <c r="BF83" s="167"/>
+      <c r="BG83" s="167"/>
+      <c r="BH83" s="167"/>
+      <c r="BI83" s="167"/>
+      <c r="BJ83" s="167"/>
+      <c r="BK83" s="167"/>
+      <c r="BL83" s="167"/>
+      <c r="BM83" s="167"/>
+      <c r="BN83" s="167"/>
+      <c r="BO83" s="167"/>
+      <c r="BP83" s="167"/>
+      <c r="BQ83" s="167"/>
+      <c r="BR83" s="167"/>
+      <c r="BS83" s="167"/>
+      <c r="BT83" s="167"/>
+      <c r="BU83" s="167"/>
+      <c r="BV83" s="167"/>
+      <c r="BW83" s="167"/>
+      <c r="BX83" s="167"/>
+      <c r="BY83" s="167"/>
+      <c r="BZ83" s="167"/>
+      <c r="CA83" s="167"/>
+      <c r="CB83" s="167"/>
+      <c r="CC83" s="167"/>
+      <c r="CD83" s="167"/>
+      <c r="CE83" s="167"/>
+      <c r="CF83" s="167"/>
+      <c r="CG83" s="167"/>
+      <c r="CH83" s="167"/>
+      <c r="CI83" s="167"/>
+      <c r="CJ83" s="167"/>
+      <c r="CK83" s="167"/>
+      <c r="CL83" s="167"/>
+      <c r="CM83" s="167"/>
+      <c r="CN83" s="167"/>
+      <c r="CO83" s="167"/>
+      <c r="CP83" s="167"/>
+      <c r="CQ83" s="167"/>
+      <c r="CR83" s="167"/>
     </row>
-    <row r="229" spans="2:96" s="307" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B229" s="310"/>
-      <c r="C229" s="308"/>
-      <c r="D229" s="308"/>
-      <c r="E229" s="306"/>
-      <c r="G229" s="308"/>
-      <c r="H229" s="309"/>
-      <c r="I229" s="308"/>
-      <c r="J229" s="308"/>
-      <c r="K229" s="308"/>
-      <c r="R229" s="306"/>
-      <c r="S229" s="305"/>
-      <c r="T229" s="304"/>
-      <c r="U229" s="303"/>
-      <c r="V229" s="302"/>
-      <c r="W229" s="302"/>
-      <c r="X229" s="302"/>
-      <c r="Y229" s="302"/>
-      <c r="Z229" s="302"/>
-      <c r="AA229" s="302"/>
-      <c r="AB229" s="302"/>
-      <c r="AC229" s="302"/>
-      <c r="AD229" s="302"/>
-      <c r="AE229" s="302"/>
-      <c r="AF229" s="302"/>
-      <c r="AG229" s="302"/>
-      <c r="AH229" s="302"/>
-      <c r="AI229" s="302"/>
-      <c r="AJ229" s="302"/>
-      <c r="AK229" s="302"/>
-      <c r="AL229" s="302"/>
-      <c r="AM229" s="302"/>
-      <c r="AN229" s="302"/>
-      <c r="AO229" s="302"/>
-      <c r="AP229" s="302"/>
-      <c r="AQ229" s="302"/>
-      <c r="AR229" s="302"/>
-      <c r="AS229" s="302"/>
-      <c r="AT229" s="302"/>
-      <c r="AU229" s="302"/>
-      <c r="AV229" s="302"/>
-      <c r="AW229" s="302"/>
-      <c r="AX229" s="302"/>
-      <c r="AY229" s="302"/>
-      <c r="AZ229" s="302"/>
-      <c r="BA229" s="302"/>
-      <c r="BB229" s="302"/>
-      <c r="BC229" s="302"/>
-      <c r="BD229" s="302"/>
-      <c r="BE229" s="302"/>
-      <c r="BF229" s="302"/>
-      <c r="BG229" s="302"/>
-      <c r="BH229" s="302"/>
-      <c r="BI229" s="302"/>
-      <c r="BJ229" s="302"/>
-      <c r="BK229" s="302"/>
-      <c r="BL229" s="302"/>
-      <c r="BM229" s="302"/>
-      <c r="BN229" s="302"/>
-      <c r="BO229" s="302"/>
-      <c r="BP229" s="302"/>
-      <c r="BQ229" s="302"/>
-      <c r="BR229" s="302"/>
-      <c r="BS229" s="302"/>
-      <c r="BT229" s="302"/>
-      <c r="BU229" s="302"/>
-      <c r="BV229" s="302"/>
-      <c r="BW229" s="302"/>
-      <c r="BX229" s="302"/>
-      <c r="BY229" s="302"/>
-      <c r="BZ229" s="302"/>
-      <c r="CA229" s="302"/>
-      <c r="CB229" s="302"/>
-      <c r="CC229" s="302"/>
-      <c r="CD229" s="302"/>
-      <c r="CE229" s="302"/>
-      <c r="CF229" s="302"/>
-      <c r="CG229" s="302"/>
-      <c r="CH229" s="302"/>
-      <c r="CI229" s="302"/>
-      <c r="CJ229" s="302"/>
-      <c r="CK229" s="302"/>
-      <c r="CL229" s="302"/>
-      <c r="CM229" s="302"/>
-      <c r="CN229" s="302"/>
-      <c r="CO229" s="302"/>
-      <c r="CP229" s="302"/>
-      <c r="CQ229" s="302"/>
-      <c r="CR229" s="302"/>
+    <row r="229" spans="2:96" s="172" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B229" s="167"/>
+      <c r="C229" s="168"/>
+      <c r="D229" s="168"/>
+      <c r="E229" s="171"/>
+      <c r="G229" s="168"/>
+      <c r="H229" s="173"/>
+      <c r="I229" s="168"/>
+      <c r="J229" s="168"/>
+      <c r="K229" s="168"/>
+      <c r="R229" s="171"/>
+      <c r="S229" s="170"/>
+      <c r="T229" s="169"/>
+      <c r="U229" s="168"/>
+      <c r="V229" s="167"/>
+      <c r="W229" s="167"/>
+      <c r="X229" s="167"/>
+      <c r="Y229" s="167"/>
+      <c r="Z229" s="167"/>
+      <c r="AA229" s="167"/>
+      <c r="AB229" s="167"/>
+      <c r="AC229" s="167"/>
+      <c r="AD229" s="167"/>
+      <c r="AE229" s="167"/>
+      <c r="AF229" s="167"/>
+      <c r="AG229" s="167"/>
+      <c r="AH229" s="167"/>
+      <c r="AI229" s="167"/>
+      <c r="AJ229" s="167"/>
+      <c r="AK229" s="167"/>
+      <c r="AL229" s="167"/>
+      <c r="AM229" s="167"/>
+      <c r="AN229" s="167"/>
+      <c r="AO229" s="167"/>
+      <c r="AP229" s="167"/>
+      <c r="AQ229" s="167"/>
+      <c r="AR229" s="167"/>
+      <c r="AS229" s="167"/>
+      <c r="AT229" s="167"/>
+      <c r="AU229" s="167"/>
+      <c r="AV229" s="167"/>
+      <c r="AW229" s="167"/>
+      <c r="AX229" s="167"/>
+      <c r="AY229" s="167"/>
+      <c r="AZ229" s="167"/>
+      <c r="BA229" s="167"/>
+      <c r="BB229" s="167"/>
+      <c r="BC229" s="167"/>
+      <c r="BD229" s="167"/>
+      <c r="BE229" s="167"/>
+      <c r="BF229" s="167"/>
+      <c r="BG229" s="167"/>
+      <c r="BH229" s="167"/>
+      <c r="BI229" s="167"/>
+      <c r="BJ229" s="167"/>
+      <c r="BK229" s="167"/>
+      <c r="BL229" s="167"/>
+      <c r="BM229" s="167"/>
+      <c r="BN229" s="167"/>
+      <c r="BO229" s="167"/>
+      <c r="BP229" s="167"/>
+      <c r="BQ229" s="167"/>
+      <c r="BR229" s="167"/>
+      <c r="BS229" s="167"/>
+      <c r="BT229" s="167"/>
+      <c r="BU229" s="167"/>
+      <c r="BV229" s="167"/>
+      <c r="BW229" s="167"/>
+      <c r="BX229" s="167"/>
+      <c r="BY229" s="167"/>
+      <c r="BZ229" s="167"/>
+      <c r="CA229" s="167"/>
+      <c r="CB229" s="167"/>
+      <c r="CC229" s="167"/>
+      <c r="CD229" s="167"/>
+      <c r="CE229" s="167"/>
+      <c r="CF229" s="167"/>
+      <c r="CG229" s="167"/>
+      <c r="CH229" s="167"/>
+      <c r="CI229" s="167"/>
+      <c r="CJ229" s="167"/>
+      <c r="CK229" s="167"/>
+      <c r="CL229" s="167"/>
+      <c r="CM229" s="167"/>
+      <c r="CN229" s="167"/>
+      <c r="CO229" s="167"/>
+      <c r="CP229" s="167"/>
+      <c r="CQ229" s="167"/>
+      <c r="CR229" s="167"/>
     </row>
-    <row r="231" spans="2:96" s="307" customFormat="1" x14ac:dyDescent="0.4">
-      <c r="B231" s="310"/>
-      <c r="C231" s="308"/>
-      <c r="D231" s="308"/>
-      <c r="E231" s="306"/>
-      <c r="G231" s="308"/>
-      <c r="H231" s="309"/>
-      <c r="I231" s="308"/>
-      <c r="J231" s="308"/>
-      <c r="K231" s="308"/>
-      <c r="R231" s="306"/>
-      <c r="S231" s="305"/>
-      <c r="T231" s="304"/>
-      <c r="U231" s="303"/>
-      <c r="V231" s="302"/>
-      <c r="W231" s="302"/>
-      <c r="X231" s="302"/>
-      <c r="Y231" s="302"/>
-      <c r="Z231" s="302"/>
-      <c r="AA231" s="302"/>
-      <c r="AB231" s="302"/>
-      <c r="AC231" s="302"/>
-      <c r="AD231" s="302"/>
-      <c r="AE231" s="302"/>
-      <c r="AF231" s="302"/>
-      <c r="AG231" s="302"/>
-      <c r="AH231" s="302"/>
-      <c r="AI231" s="302"/>
-      <c r="AJ231" s="302"/>
-      <c r="AK231" s="302"/>
-      <c r="AL231" s="302"/>
-      <c r="AM231" s="302"/>
-      <c r="AN231" s="302"/>
-      <c r="AO231" s="302"/>
-      <c r="AP231" s="302"/>
-      <c r="AQ231" s="302"/>
-      <c r="AR231" s="302"/>
-      <c r="AS231" s="302"/>
-      <c r="AT231" s="302"/>
-      <c r="AU231" s="302"/>
-      <c r="AV231" s="302"/>
-      <c r="AW231" s="302"/>
-      <c r="AX231" s="302"/>
-      <c r="AY231" s="302"/>
-      <c r="AZ231" s="302"/>
-      <c r="BA231" s="302"/>
-      <c r="BB231" s="302"/>
-      <c r="BC231" s="302"/>
-      <c r="BD231" s="302"/>
-      <c r="BE231" s="302"/>
-      <c r="BF231" s="302"/>
-      <c r="BG231" s="302"/>
-      <c r="BH231" s="302"/>
-      <c r="BI231" s="302"/>
-      <c r="BJ231" s="302"/>
-      <c r="BK231" s="302"/>
-      <c r="BL231" s="302"/>
-      <c r="BM231" s="302"/>
-      <c r="BN231" s="302"/>
-      <c r="BO231" s="302"/>
-      <c r="BP231" s="302"/>
-      <c r="BQ231" s="302"/>
-      <c r="BR231" s="302"/>
-      <c r="BS231" s="302"/>
-      <c r="BT231" s="302"/>
-      <c r="BU231" s="302"/>
-      <c r="BV231" s="302"/>
-      <c r="BW231" s="302"/>
-      <c r="BX231" s="302"/>
-      <c r="BY231" s="302"/>
-      <c r="BZ231" s="302"/>
-      <c r="CA231" s="302"/>
-      <c r="CB231" s="302"/>
-      <c r="CC231" s="302"/>
-      <c r="CD231" s="302"/>
-      <c r="CE231" s="302"/>
-      <c r="CF231" s="302"/>
-      <c r="CG231" s="302"/>
-      <c r="CH231" s="302"/>
-      <c r="CI231" s="302"/>
-      <c r="CJ231" s="302"/>
-      <c r="CK231" s="302"/>
-      <c r="CL231" s="302"/>
-      <c r="CM231" s="302"/>
-      <c r="CN231" s="302"/>
-      <c r="CO231" s="302"/>
-      <c r="CP231" s="302"/>
-      <c r="CQ231" s="302"/>
-      <c r="CR231" s="302"/>
+    <row r="231" spans="2:96" s="172" customFormat="1" x14ac:dyDescent="0.4">
+      <c r="B231" s="167"/>
+      <c r="C231" s="168"/>
+      <c r="D231" s="168"/>
+      <c r="E231" s="171"/>
+      <c r="G231" s="168"/>
+      <c r="H231" s="173"/>
+      <c r="I231" s="168"/>
+      <c r="J231" s="168"/>
+      <c r="K231" s="168"/>
+      <c r="R231" s="171"/>
+      <c r="S231" s="170"/>
+      <c r="T231" s="169"/>
+      <c r="U231" s="168"/>
+      <c r="V231" s="167"/>
+      <c r="W231" s="167"/>
+      <c r="X231" s="167"/>
+      <c r="Y231" s="167"/>
+      <c r="Z231" s="167"/>
+      <c r="AA231" s="167"/>
+      <c r="AB231" s="167"/>
+      <c r="AC231" s="167"/>
+      <c r="AD231" s="167"/>
+      <c r="AE231" s="167"/>
+      <c r="AF231" s="167"/>
+      <c r="AG231" s="167"/>
+      <c r="AH231" s="167"/>
+      <c r="AI231" s="167"/>
+      <c r="AJ231" s="167"/>
+      <c r="AK231" s="167"/>
+      <c r="AL231" s="167"/>
+      <c r="AM231" s="167"/>
+      <c r="AN231" s="167"/>
+      <c r="AO231" s="167"/>
+      <c r="AP231" s="167"/>
+      <c r="AQ231" s="167"/>
+      <c r="AR231" s="167"/>
+      <c r="AS231" s="167"/>
+      <c r="AT231" s="167"/>
+      <c r="AU231" s="167"/>
+      <c r="AV231" s="167"/>
+      <c r="AW231" s="167"/>
+      <c r="AX231" s="167"/>
+      <c r="AY231" s="167"/>
+      <c r="AZ231" s="167"/>
+      <c r="BA231" s="167"/>
+      <c r="BB231" s="167"/>
+      <c r="BC231" s="167"/>
+      <c r="BD231" s="167"/>
+      <c r="BE231" s="167"/>
+      <c r="BF231" s="167"/>
+      <c r="BG231" s="167"/>
+      <c r="BH231" s="167"/>
+      <c r="BI231" s="167"/>
+      <c r="BJ231" s="167"/>
+      <c r="BK231" s="167"/>
+      <c r="BL231" s="167"/>
+      <c r="BM231" s="167"/>
+      <c r="BN231" s="167"/>
+      <c r="BO231" s="167"/>
+      <c r="BP231" s="167"/>
+      <c r="BQ231" s="167"/>
+      <c r="BR231" s="167"/>
+      <c r="BS231" s="167"/>
+      <c r="BT231" s="167"/>
+      <c r="BU231" s="167"/>
+      <c r="BV231" s="167"/>
+      <c r="BW231" s="167"/>
+      <c r="BX231" s="167"/>
+      <c r="BY231" s="167"/>
+      <c r="BZ231" s="167"/>
+      <c r="CA231" s="167"/>
+      <c r="CB231" s="167"/>
+      <c r="CC231" s="167"/>
+      <c r="CD231" s="167"/>
+      <c r="CE231" s="167"/>
+      <c r="CF231" s="167"/>
+      <c r="CG231" s="167"/>
+      <c r="CH231" s="167"/>
+      <c r="CI231" s="167"/>
+      <c r="CJ231" s="167"/>
+      <c r="CK231" s="167"/>
+      <c r="CL231" s="167"/>
+      <c r="CM231" s="167"/>
+      <c r="CN231" s="167"/>
+      <c r="CO231" s="167"/>
+      <c r="CP231" s="167"/>
+      <c r="CQ231" s="167"/>
+      <c r="CR231" s="167"/>
     </row>
   </sheetData>
-  <autoFilter ref="B2:CG2"/>
+  <autoFilter ref="B2:CG2" xr:uid="{00000000-0009-0000-0000-000001000000}"/>
   <phoneticPr fontId="2" type="noConversion"/>
   <printOptions horizontalCentered="1"/>
   <pageMargins left="0" right="0" top="0.39370078740157483" bottom="0.31496062992125984" header="0.19685039370078741" footer="0.19685039370078741"/>

</xml_diff>